<commit_message>
Balance Modif with I&E
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -8,35 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenny\Documents\Kenny\Coding\NSB-AlgoProg-Group-Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A14D8D1-A5B9-4756-8B66-5C352A71554B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3317C8ED-1E1A-4654-B15C-1E5BB19C08D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Index</t>
   </si>
   <si>
     <t>Entry</t>
+  </si>
+  <si>
+    <t>Date of Transaction</t>
   </si>
   <si>
     <t>I/E</t>
@@ -51,6 +43,18 @@
     <t>Delivery</t>
   </si>
   <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Date/Time of Modification</t>
+  </si>
+  <si>
+    <t>Other Info</t>
+  </si>
+  <si>
+    <t>Status/Value</t>
+  </si>
+  <si>
     <t>SALARY</t>
   </si>
   <si>
@@ -58,6 +62,9 @@
   </si>
   <si>
     <t>income</t>
+  </si>
+  <si>
+    <t>Balance</t>
   </si>
   <si>
     <t>WATER</t>
@@ -69,25 +76,22 @@
     <t>expense</t>
   </si>
   <si>
-    <t>ID</t>
+    <t>Budget Bal.</t>
   </si>
   <si>
-    <t>Date of Transaction</t>
+    <t>COMMISSION</t>
   </si>
   <si>
-    <t>Date/Time of Modification</t>
+    <t>2024-10-14</t>
   </si>
   <si>
-    <t>Other Info</t>
+    <t>INCOME</t>
   </si>
   <si>
-    <t>Status/Value</t>
+    <t>000003</t>
   </si>
   <si>
-    <t>Balance</t>
-  </si>
-  <si>
-    <t>Budget Bal.</t>
+    <t>2024-10-14 / 13:21:50</t>
   </si>
   <si>
     <t>Total Exp.</t>
@@ -97,8 +101,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="165" formatCode="000000"/>
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -152,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -174,6 +180,28 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,20 +518,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="5.6796875" customWidth="1"/>
     <col min="2" max="2" width="20.90625" customWidth="1"/>
-    <col min="3" max="3" width="19.04296875" customWidth="1"/>
+    <col min="3" max="3" width="19.04296875" style="17" customWidth="1"/>
     <col min="4" max="4" width="14.2265625" customWidth="1"/>
     <col min="5" max="5" width="13.90625" style="7" customWidth="1"/>
     <col min="6" max="6" width="16.90625" customWidth="1"/>
     <col min="7" max="7" width="14.08984375" customWidth="1"/>
-    <col min="8" max="8" width="14.26953125" customWidth="1"/>
+    <col min="8" max="8" width="14.26953125" style="13" customWidth="1"/>
     <col min="9" max="9" width="25.26953125" customWidth="1"/>
     <col min="11" max="11" width="13.6328125" customWidth="1"/>
     <col min="12" max="12" width="12.953125" customWidth="1"/>
@@ -516,33 +544,33 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
+      <c r="C1" s="18" t="s">
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
@@ -553,28 +581,30 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="C2" s="14"/>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E2" s="5">
         <v>35000</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H2" s="2"/>
+      <c r="H2" s="9"/>
       <c r="I2" s="2"/>
       <c r="J2" s="3"/>
       <c r="K2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="L2" s="5">
+        <v>0</v>
+      </c>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
@@ -584,28 +614,30 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="C3" s="14"/>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E3" s="5">
         <v>28000</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G3" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H3" s="2"/>
+      <c r="H3" s="10"/>
       <c r="I3" s="2"/>
       <c r="J3" s="3"/>
       <c r="K3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="2"/>
+      <c r="L3" s="5">
+        <v>0</v>
+      </c>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
@@ -614,19 +646,35 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1000</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="J4" s="3"/>
       <c r="K4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L4" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="L4" s="5"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
@@ -636,12 +684,12 @@
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="C5" s="14"/>
       <c r="D5" s="2"/>
       <c r="E5" s="5"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="H5" s="10"/>
       <c r="I5" s="2"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -655,12 +703,12 @@
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="C6" s="14"/>
       <c r="D6" s="2"/>
       <c r="E6" s="5"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="H6" s="10"/>
       <c r="I6" s="2"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -674,12 +722,12 @@
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="C7" s="14"/>
       <c r="D7" s="2"/>
       <c r="E7" s="5"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="H7" s="10"/>
       <c r="I7" s="2"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -693,11 +741,11 @@
         <v>7</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="8"/>
+      <c r="C8" s="15"/>
       <c r="E8" s="5"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
+      <c r="H8" s="11"/>
       <c r="I8" s="8"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -711,12 +759,12 @@
         <v>8</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="C9" s="14"/>
       <c r="D9" s="2"/>
       <c r="E9" s="5"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="H9" s="10"/>
       <c r="I9" s="2"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -730,12 +778,12 @@
         <v>9</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="C10" s="14"/>
       <c r="D10" s="2"/>
       <c r="E10" s="5"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="H10" s="10"/>
       <c r="I10" s="2"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -749,12 +797,12 @@
         <v>10</v>
       </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="C11" s="14"/>
       <c r="D11" s="2"/>
       <c r="E11" s="5"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="H11" s="10"/>
       <c r="I11" s="2"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -768,12 +816,12 @@
         <v>11</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="C12" s="14"/>
       <c r="D12" s="2"/>
       <c r="E12" s="5"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="H12" s="10"/>
       <c r="I12" s="2"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -787,12 +835,12 @@
         <v>12</v>
       </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="2"/>
       <c r="E13" s="5"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="H13" s="10"/>
       <c r="I13" s="2"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -806,12 +854,12 @@
         <v>13</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="C14" s="14"/>
       <c r="D14" s="2"/>
       <c r="E14" s="5"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="H14" s="10"/>
       <c r="I14" s="2"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -825,12 +873,12 @@
         <v>14</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="C15" s="14"/>
       <c r="D15" s="2"/>
       <c r="E15" s="5"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="H15" s="10"/>
       <c r="I15" s="2"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -844,12 +892,12 @@
         <v>15</v>
       </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="C16" s="14"/>
       <c r="D16" s="2"/>
       <c r="E16" s="5"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="H16" s="10"/>
       <c r="I16" s="2"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -863,12 +911,12 @@
         <v>16</v>
       </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="C17" s="14"/>
       <c r="D17" s="2"/>
       <c r="E17" s="5"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="H17" s="10"/>
       <c r="I17" s="2"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -882,12 +930,12 @@
         <v>17</v>
       </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="C18" s="14"/>
       <c r="D18" s="2"/>
       <c r="E18" s="5"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="H18" s="10"/>
       <c r="I18" s="2"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -901,12 +949,12 @@
         <v>18</v>
       </c>
       <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="C19" s="14"/>
       <c r="D19" s="2"/>
       <c r="E19" s="5"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="H19" s="10"/>
       <c r="I19" s="2"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -920,12 +968,12 @@
         <v>19</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="C20" s="14"/>
       <c r="D20" s="2"/>
       <c r="E20" s="5"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="H20" s="10"/>
       <c r="I20" s="2"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -939,12 +987,12 @@
         <v>20</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="C21" s="14"/>
       <c r="D21" s="2"/>
       <c r="E21" s="5"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+      <c r="H21" s="10"/>
       <c r="I21" s="2"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -958,12 +1006,12 @@
         <v>21</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="C22" s="14"/>
       <c r="D22" s="2"/>
       <c r="E22" s="5"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="H22" s="10"/>
       <c r="I22" s="2"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -977,12 +1025,12 @@
         <v>22</v>
       </c>
       <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+      <c r="C23" s="14"/>
       <c r="D23" s="2"/>
       <c r="E23" s="5"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="H23" s="10"/>
       <c r="I23" s="2"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -996,12 +1044,12 @@
         <v>23</v>
       </c>
       <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
+      <c r="C24" s="14"/>
       <c r="D24" s="2"/>
       <c r="E24" s="5"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
+      <c r="H24" s="10"/>
       <c r="I24" s="2"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -1015,12 +1063,12 @@
         <v>24</v>
       </c>
       <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
+      <c r="C25" s="14"/>
       <c r="D25" s="2"/>
       <c r="E25" s="5"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
+      <c r="H25" s="10"/>
       <c r="I25" s="2"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -1034,12 +1082,12 @@
         <v>25</v>
       </c>
       <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+      <c r="C26" s="14"/>
       <c r="D26" s="2"/>
       <c r="E26" s="5"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
+      <c r="H26" s="10"/>
       <c r="I26" s="2"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
@@ -1053,12 +1101,12 @@
         <v>26</v>
       </c>
       <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
+      <c r="C27" s="14"/>
       <c r="D27" s="2"/>
       <c r="E27" s="5"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
+      <c r="H27" s="10"/>
       <c r="I27" s="2"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
@@ -1072,12 +1120,12 @@
         <v>27</v>
       </c>
       <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+      <c r="C28" s="14"/>
       <c r="D28" s="2"/>
       <c r="E28" s="5"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
+      <c r="H28" s="10"/>
       <c r="I28" s="2"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
@@ -1091,12 +1139,12 @@
         <v>28</v>
       </c>
       <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+      <c r="C29" s="14"/>
       <c r="D29" s="2"/>
       <c r="E29" s="5"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
+      <c r="H29" s="10"/>
       <c r="I29" s="2"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -1110,12 +1158,12 @@
         <v>29</v>
       </c>
       <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
+      <c r="C30" s="14"/>
       <c r="D30" s="2"/>
       <c r="E30" s="5"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
+      <c r="H30" s="10"/>
       <c r="I30" s="2"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -1129,12 +1177,12 @@
         <v>30</v>
       </c>
       <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
+      <c r="C31" s="14"/>
       <c r="D31" s="2"/>
       <c r="E31" s="5"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
+      <c r="H31" s="10"/>
       <c r="I31" s="2"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
@@ -1148,12 +1196,12 @@
         <v>31</v>
       </c>
       <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
+      <c r="C32" s="14"/>
       <c r="D32" s="2"/>
       <c r="E32" s="5"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
+      <c r="H32" s="10"/>
       <c r="I32" s="2"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
@@ -1167,12 +1215,12 @@
         <v>32</v>
       </c>
       <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="C33" s="14"/>
       <c r="D33" s="2"/>
       <c r="E33" s="5"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
+      <c r="H33" s="10"/>
       <c r="I33" s="2"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
@@ -1186,12 +1234,12 @@
         <v>33</v>
       </c>
       <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
+      <c r="C34" s="14"/>
       <c r="D34" s="2"/>
       <c r="E34" s="5"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
+      <c r="H34" s="10"/>
       <c r="I34" s="2"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
@@ -1205,12 +1253,12 @@
         <v>34</v>
       </c>
       <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
+      <c r="C35" s="14"/>
       <c r="D35" s="2"/>
       <c r="E35" s="5"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
+      <c r="H35" s="10"/>
       <c r="I35" s="2"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
@@ -1224,12 +1272,12 @@
         <v>35</v>
       </c>
       <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
+      <c r="C36" s="14"/>
       <c r="D36" s="2"/>
       <c r="E36" s="5"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
+      <c r="H36" s="10"/>
       <c r="I36" s="2"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
@@ -1243,12 +1291,12 @@
         <v>36</v>
       </c>
       <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
+      <c r="C37" s="14"/>
       <c r="D37" s="2"/>
       <c r="E37" s="5"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
+      <c r="H37" s="10"/>
       <c r="I37" s="2"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
@@ -1262,12 +1310,12 @@
         <v>37</v>
       </c>
       <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
+      <c r="C38" s="14"/>
       <c r="D38" s="2"/>
       <c r="E38" s="5"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
+      <c r="H38" s="10"/>
       <c r="I38" s="2"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
@@ -1281,12 +1329,12 @@
         <v>38</v>
       </c>
       <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
+      <c r="C39" s="14"/>
       <c r="D39" s="2"/>
       <c r="E39" s="5"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
+      <c r="H39" s="10"/>
       <c r="I39" s="2"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
@@ -1300,12 +1348,12 @@
         <v>39</v>
       </c>
       <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
+      <c r="C40" s="14"/>
       <c r="D40" s="2"/>
       <c r="E40" s="5"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
+      <c r="H40" s="10"/>
       <c r="I40" s="2"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
@@ -1319,12 +1367,12 @@
         <v>40</v>
       </c>
       <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
+      <c r="C41" s="14"/>
       <c r="D41" s="2"/>
       <c r="E41" s="5"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
+      <c r="H41" s="10"/>
       <c r="I41" s="2"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
@@ -1338,12 +1386,12 @@
         <v>41</v>
       </c>
       <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
+      <c r="C42" s="14"/>
       <c r="D42" s="2"/>
       <c r="E42" s="5"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
+      <c r="H42" s="10"/>
       <c r="I42" s="2"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
@@ -1357,12 +1405,12 @@
         <v>42</v>
       </c>
       <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
+      <c r="C43" s="14"/>
       <c r="D43" s="2"/>
       <c r="E43" s="5"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
+      <c r="H43" s="10"/>
       <c r="I43" s="2"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
@@ -1376,12 +1424,12 @@
         <v>43</v>
       </c>
       <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
+      <c r="C44" s="14"/>
       <c r="D44" s="2"/>
       <c r="E44" s="5"/>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
+      <c r="H44" s="10"/>
       <c r="I44" s="2"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
@@ -1395,12 +1443,12 @@
         <v>44</v>
       </c>
       <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
+      <c r="C45" s="14"/>
       <c r="D45" s="2"/>
       <c r="E45" s="5"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
+      <c r="H45" s="10"/>
       <c r="I45" s="2"/>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
@@ -1414,12 +1462,12 @@
         <v>45</v>
       </c>
       <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
+      <c r="C46" s="14"/>
       <c r="D46" s="2"/>
       <c r="E46" s="5"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
+      <c r="H46" s="10"/>
       <c r="I46" s="2"/>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
@@ -1433,12 +1481,12 @@
         <v>46</v>
       </c>
       <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
+      <c r="C47" s="14"/>
       <c r="D47" s="2"/>
       <c r="E47" s="5"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
+      <c r="H47" s="10"/>
       <c r="I47" s="2"/>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
@@ -1452,12 +1500,12 @@
         <v>47</v>
       </c>
       <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
+      <c r="C48" s="14"/>
       <c r="D48" s="2"/>
       <c r="E48" s="5"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
+      <c r="H48" s="10"/>
       <c r="I48" s="2"/>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
@@ -1471,12 +1519,12 @@
         <v>48</v>
       </c>
       <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
+      <c r="C49" s="14"/>
       <c r="D49" s="2"/>
       <c r="E49" s="5"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
+      <c r="H49" s="10"/>
       <c r="I49" s="2"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
@@ -1490,12 +1538,12 @@
         <v>49</v>
       </c>
       <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
+      <c r="C50" s="14"/>
       <c r="D50" s="2"/>
       <c r="E50" s="5"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
+      <c r="H50" s="10"/>
       <c r="I50" s="2"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
@@ -1509,12 +1557,12 @@
         <v>50</v>
       </c>
       <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
+      <c r="C51" s="14"/>
       <c r="D51" s="2"/>
       <c r="E51" s="5"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
+      <c r="H51" s="10"/>
       <c r="I51" s="2"/>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
@@ -1528,12 +1576,12 @@
         <v>51</v>
       </c>
       <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
+      <c r="C52" s="14"/>
       <c r="D52" s="2"/>
       <c r="E52" s="5"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
+      <c r="H52" s="10"/>
       <c r="I52" s="2"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
@@ -1547,12 +1595,12 @@
         <v>52</v>
       </c>
       <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
+      <c r="C53" s="14"/>
       <c r="D53" s="2"/>
       <c r="E53" s="5"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
+      <c r="H53" s="10"/>
       <c r="I53" s="2"/>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
@@ -1566,12 +1614,12 @@
         <v>53</v>
       </c>
       <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
+      <c r="C54" s="14"/>
       <c r="D54" s="2"/>
       <c r="E54" s="5"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
+      <c r="H54" s="10"/>
       <c r="I54" s="2"/>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
@@ -1585,12 +1633,12 @@
         <v>54</v>
       </c>
       <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
+      <c r="C55" s="14"/>
       <c r="D55" s="2"/>
       <c r="E55" s="5"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
+      <c r="H55" s="10"/>
       <c r="I55" s="2"/>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
@@ -1604,12 +1652,12 @@
         <v>55</v>
       </c>
       <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
+      <c r="C56" s="14"/>
       <c r="D56" s="2"/>
       <c r="E56" s="5"/>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
+      <c r="H56" s="10"/>
       <c r="I56" s="2"/>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
@@ -1623,12 +1671,12 @@
         <v>56</v>
       </c>
       <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
+      <c r="C57" s="14"/>
       <c r="D57" s="2"/>
       <c r="E57" s="5"/>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
-      <c r="H57" s="2"/>
+      <c r="H57" s="10"/>
       <c r="I57" s="2"/>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
@@ -1642,12 +1690,12 @@
         <v>57</v>
       </c>
       <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
+      <c r="C58" s="14"/>
       <c r="D58" s="2"/>
       <c r="E58" s="5"/>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
-      <c r="H58" s="2"/>
+      <c r="H58" s="10"/>
       <c r="I58" s="2"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
@@ -1661,12 +1709,12 @@
         <v>58</v>
       </c>
       <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
+      <c r="C59" s="14"/>
       <c r="D59" s="2"/>
       <c r="E59" s="5"/>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
-      <c r="H59" s="2"/>
+      <c r="H59" s="10"/>
       <c r="I59" s="2"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
@@ -1680,12 +1728,12 @@
         <v>59</v>
       </c>
       <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
+      <c r="C60" s="14"/>
       <c r="D60" s="2"/>
       <c r="E60" s="5"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
+      <c r="H60" s="10"/>
       <c r="I60" s="2"/>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
@@ -1699,12 +1747,12 @@
         <v>60</v>
       </c>
       <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
+      <c r="C61" s="14"/>
       <c r="D61" s="2"/>
       <c r="E61" s="5"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
+      <c r="H61" s="10"/>
       <c r="I61" s="2"/>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
@@ -1718,12 +1766,12 @@
         <v>61</v>
       </c>
       <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
+      <c r="C62" s="14"/>
       <c r="D62" s="2"/>
       <c r="E62" s="5"/>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
-      <c r="H62" s="2"/>
+      <c r="H62" s="10"/>
       <c r="I62" s="2"/>
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
@@ -1737,12 +1785,12 @@
         <v>62</v>
       </c>
       <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
+      <c r="C63" s="14"/>
       <c r="D63" s="2"/>
       <c r="E63" s="5"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
+      <c r="H63" s="10"/>
       <c r="I63" s="2"/>
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
@@ -1756,12 +1804,12 @@
         <v>63</v>
       </c>
       <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
+      <c r="C64" s="14"/>
       <c r="D64" s="2"/>
       <c r="E64" s="5"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
+      <c r="H64" s="10"/>
       <c r="I64" s="2"/>
       <c r="J64" s="3"/>
       <c r="K64" s="3"/>
@@ -1775,12 +1823,12 @@
         <v>64</v>
       </c>
       <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
+      <c r="C65" s="14"/>
       <c r="D65" s="2"/>
       <c r="E65" s="5"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
+      <c r="H65" s="10"/>
       <c r="I65" s="2"/>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
@@ -1794,12 +1842,12 @@
         <v>65</v>
       </c>
       <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
+      <c r="C66" s="14"/>
       <c r="D66" s="2"/>
       <c r="E66" s="5"/>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
+      <c r="H66" s="10"/>
       <c r="I66" s="2"/>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
@@ -1813,12 +1861,12 @@
         <v>66</v>
       </c>
       <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
+      <c r="C67" s="14"/>
       <c r="D67" s="2"/>
       <c r="E67" s="5"/>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
+      <c r="H67" s="10"/>
       <c r="I67" s="2"/>
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
@@ -1832,12 +1880,12 @@
         <v>67</v>
       </c>
       <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
+      <c r="C68" s="14"/>
       <c r="D68" s="2"/>
       <c r="E68" s="5"/>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
-      <c r="H68" s="2"/>
+      <c r="H68" s="10"/>
       <c r="I68" s="2"/>
       <c r="J68" s="3"/>
       <c r="K68" s="3"/>
@@ -1851,12 +1899,12 @@
         <v>68</v>
       </c>
       <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
+      <c r="C69" s="14"/>
       <c r="D69" s="2"/>
       <c r="E69" s="5"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
-      <c r="H69" s="2"/>
+      <c r="H69" s="10"/>
       <c r="I69" s="2"/>
       <c r="J69" s="3"/>
       <c r="K69" s="3"/>
@@ -1870,12 +1918,12 @@
         <v>69</v>
       </c>
       <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
+      <c r="C70" s="14"/>
       <c r="D70" s="2"/>
       <c r="E70" s="5"/>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
-      <c r="H70" s="2"/>
+      <c r="H70" s="10"/>
       <c r="I70" s="2"/>
       <c r="J70" s="3"/>
       <c r="K70" s="3"/>
@@ -1889,12 +1937,12 @@
         <v>70</v>
       </c>
       <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
+      <c r="C71" s="14"/>
       <c r="D71" s="2"/>
       <c r="E71" s="5"/>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
-      <c r="H71" s="2"/>
+      <c r="H71" s="10"/>
       <c r="I71" s="2"/>
       <c r="J71" s="3"/>
       <c r="K71" s="3"/>
@@ -1908,12 +1956,12 @@
         <v>71</v>
       </c>
       <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
+      <c r="C72" s="14"/>
       <c r="D72" s="2"/>
       <c r="E72" s="5"/>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
-      <c r="H72" s="2"/>
+      <c r="H72" s="10"/>
       <c r="I72" s="2"/>
       <c r="J72" s="3"/>
       <c r="K72" s="3"/>
@@ -1927,12 +1975,12 @@
         <v>72</v>
       </c>
       <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
+      <c r="C73" s="14"/>
       <c r="D73" s="2"/>
       <c r="E73" s="5"/>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
-      <c r="H73" s="2"/>
+      <c r="H73" s="10"/>
       <c r="I73" s="2"/>
       <c r="J73" s="3"/>
       <c r="K73" s="3"/>
@@ -1946,12 +1994,12 @@
         <v>73</v>
       </c>
       <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
+      <c r="C74" s="14"/>
       <c r="D74" s="2"/>
       <c r="E74" s="5"/>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
-      <c r="H74" s="2"/>
+      <c r="H74" s="10"/>
       <c r="I74" s="2"/>
       <c r="J74" s="3"/>
       <c r="K74" s="3"/>
@@ -1965,12 +2013,12 @@
         <v>74</v>
       </c>
       <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
+      <c r="C75" s="14"/>
       <c r="D75" s="2"/>
       <c r="E75" s="5"/>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
-      <c r="H75" s="2"/>
+      <c r="H75" s="10"/>
       <c r="I75" s="2"/>
       <c r="J75" s="3"/>
       <c r="K75" s="3"/>
@@ -1984,12 +2032,12 @@
         <v>75</v>
       </c>
       <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
+      <c r="C76" s="14"/>
       <c r="D76" s="2"/>
       <c r="E76" s="5"/>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
-      <c r="H76" s="2"/>
+      <c r="H76" s="10"/>
       <c r="I76" s="2"/>
       <c r="J76" s="3"/>
       <c r="K76" s="3"/>
@@ -2003,12 +2051,12 @@
         <v>76</v>
       </c>
       <c r="B77" s="2"/>
-      <c r="C77" s="2"/>
+      <c r="C77" s="14"/>
       <c r="D77" s="2"/>
       <c r="E77" s="5"/>
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
-      <c r="H77" s="2"/>
+      <c r="H77" s="10"/>
       <c r="I77" s="2"/>
       <c r="J77" s="3"/>
       <c r="K77" s="3"/>
@@ -2022,12 +2070,12 @@
         <v>77</v>
       </c>
       <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
+      <c r="C78" s="14"/>
       <c r="D78" s="2"/>
       <c r="E78" s="5"/>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
-      <c r="H78" s="2"/>
+      <c r="H78" s="10"/>
       <c r="I78" s="2"/>
       <c r="J78" s="3"/>
       <c r="K78" s="3"/>
@@ -2041,12 +2089,12 @@
         <v>78</v>
       </c>
       <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
+      <c r="C79" s="14"/>
       <c r="D79" s="2"/>
       <c r="E79" s="5"/>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
-      <c r="H79" s="2"/>
+      <c r="H79" s="10"/>
       <c r="I79" s="2"/>
       <c r="J79" s="3"/>
       <c r="K79" s="3"/>
@@ -2060,12 +2108,12 @@
         <v>79</v>
       </c>
       <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
+      <c r="C80" s="14"/>
       <c r="D80" s="2"/>
       <c r="E80" s="5"/>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
-      <c r="H80" s="2"/>
+      <c r="H80" s="10"/>
       <c r="I80" s="2"/>
       <c r="J80" s="3"/>
       <c r="K80" s="3"/>
@@ -2079,12 +2127,12 @@
         <v>80</v>
       </c>
       <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
+      <c r="C81" s="14"/>
       <c r="D81" s="2"/>
       <c r="E81" s="5"/>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
-      <c r="H81" s="2"/>
+      <c r="H81" s="10"/>
       <c r="I81" s="2"/>
       <c r="J81" s="3"/>
       <c r="K81" s="3"/>
@@ -2098,12 +2146,12 @@
         <v>81</v>
       </c>
       <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
+      <c r="C82" s="14"/>
       <c r="D82" s="2"/>
       <c r="E82" s="5"/>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
-      <c r="H82" s="2"/>
+      <c r="H82" s="10"/>
       <c r="I82" s="2"/>
       <c r="J82" s="3"/>
       <c r="K82" s="3"/>
@@ -2117,12 +2165,12 @@
         <v>82</v>
       </c>
       <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
+      <c r="C83" s="14"/>
       <c r="D83" s="2"/>
       <c r="E83" s="5"/>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
-      <c r="H83" s="2"/>
+      <c r="H83" s="10"/>
       <c r="I83" s="2"/>
       <c r="J83" s="3"/>
       <c r="K83" s="3"/>
@@ -2136,12 +2184,12 @@
         <v>83</v>
       </c>
       <c r="B84" s="2"/>
-      <c r="C84" s="2"/>
+      <c r="C84" s="14"/>
       <c r="D84" s="2"/>
       <c r="E84" s="5"/>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
-      <c r="H84" s="2"/>
+      <c r="H84" s="10"/>
       <c r="I84" s="2"/>
       <c r="J84" s="3"/>
       <c r="K84" s="3"/>
@@ -2155,12 +2203,12 @@
         <v>84</v>
       </c>
       <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
+      <c r="C85" s="14"/>
       <c r="D85" s="2"/>
       <c r="E85" s="5"/>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
-      <c r="H85" s="2"/>
+      <c r="H85" s="10"/>
       <c r="I85" s="2"/>
       <c r="J85" s="3"/>
       <c r="K85" s="3"/>
@@ -2174,12 +2222,12 @@
         <v>85</v>
       </c>
       <c r="B86" s="2"/>
-      <c r="C86" s="2"/>
+      <c r="C86" s="14"/>
       <c r="D86" s="2"/>
       <c r="E86" s="5"/>
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
-      <c r="H86" s="2"/>
+      <c r="H86" s="10"/>
       <c r="I86" s="2"/>
       <c r="J86" s="3"/>
       <c r="K86" s="3"/>
@@ -2193,12 +2241,12 @@
         <v>86</v>
       </c>
       <c r="B87" s="2"/>
-      <c r="C87" s="2"/>
+      <c r="C87" s="14"/>
       <c r="D87" s="2"/>
       <c r="E87" s="5"/>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
-      <c r="H87" s="2"/>
+      <c r="H87" s="10"/>
       <c r="I87" s="2"/>
       <c r="J87" s="3"/>
       <c r="K87" s="3"/>
@@ -2212,12 +2260,12 @@
         <v>87</v>
       </c>
       <c r="B88" s="2"/>
-      <c r="C88" s="2"/>
+      <c r="C88" s="14"/>
       <c r="D88" s="2"/>
       <c r="E88" s="5"/>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
-      <c r="H88" s="2"/>
+      <c r="H88" s="10"/>
       <c r="I88" s="2"/>
       <c r="J88" s="3"/>
       <c r="K88" s="3"/>
@@ -2231,12 +2279,12 @@
         <v>88</v>
       </c>
       <c r="B89" s="2"/>
-      <c r="C89" s="2"/>
+      <c r="C89" s="14"/>
       <c r="D89" s="2"/>
       <c r="E89" s="5"/>
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
-      <c r="H89" s="2"/>
+      <c r="H89" s="10"/>
       <c r="I89" s="2"/>
       <c r="J89" s="3"/>
       <c r="K89" s="3"/>
@@ -2250,12 +2298,12 @@
         <v>89</v>
       </c>
       <c r="B90" s="2"/>
-      <c r="C90" s="2"/>
+      <c r="C90" s="14"/>
       <c r="D90" s="2"/>
       <c r="E90" s="5"/>
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
-      <c r="H90" s="2"/>
+      <c r="H90" s="10"/>
       <c r="I90" s="2"/>
       <c r="J90" s="3"/>
       <c r="K90" s="3"/>
@@ -2269,12 +2317,12 @@
         <v>90</v>
       </c>
       <c r="B91" s="2"/>
-      <c r="C91" s="2"/>
+      <c r="C91" s="14"/>
       <c r="D91" s="2"/>
       <c r="E91" s="5"/>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
-      <c r="H91" s="2"/>
+      <c r="H91" s="10"/>
       <c r="I91" s="2"/>
       <c r="J91" s="3"/>
       <c r="K91" s="3"/>
@@ -2288,12 +2336,12 @@
         <v>91</v>
       </c>
       <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
+      <c r="C92" s="14"/>
       <c r="D92" s="2"/>
       <c r="E92" s="5"/>
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
-      <c r="H92" s="2"/>
+      <c r="H92" s="10"/>
       <c r="I92" s="2"/>
       <c r="J92" s="3"/>
       <c r="K92" s="3"/>
@@ -2307,12 +2355,12 @@
         <v>92</v>
       </c>
       <c r="B93" s="2"/>
-      <c r="C93" s="2"/>
+      <c r="C93" s="14"/>
       <c r="D93" s="2"/>
       <c r="E93" s="5"/>
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
-      <c r="H93" s="2"/>
+      <c r="H93" s="10"/>
       <c r="I93" s="2"/>
       <c r="J93" s="3"/>
       <c r="K93" s="3"/>
@@ -2326,12 +2374,12 @@
         <v>93</v>
       </c>
       <c r="B94" s="2"/>
-      <c r="C94" s="2"/>
+      <c r="C94" s="14"/>
       <c r="D94" s="2"/>
       <c r="E94" s="5"/>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
-      <c r="H94" s="2"/>
+      <c r="H94" s="10"/>
       <c r="I94" s="2"/>
       <c r="J94" s="3"/>
       <c r="K94" s="3"/>
@@ -2345,12 +2393,12 @@
         <v>94</v>
       </c>
       <c r="B95" s="2"/>
-      <c r="C95" s="2"/>
+      <c r="C95" s="14"/>
       <c r="D95" s="2"/>
       <c r="E95" s="5"/>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
-      <c r="H95" s="2"/>
+      <c r="H95" s="10"/>
       <c r="I95" s="2"/>
       <c r="J95" s="3"/>
       <c r="K95" s="3"/>
@@ -2364,12 +2412,12 @@
         <v>95</v>
       </c>
       <c r="B96" s="2"/>
-      <c r="C96" s="2"/>
+      <c r="C96" s="14"/>
       <c r="D96" s="2"/>
       <c r="E96" s="5"/>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
-      <c r="H96" s="2"/>
+      <c r="H96" s="10"/>
       <c r="I96" s="2"/>
       <c r="J96" s="3"/>
       <c r="K96" s="3"/>
@@ -2383,12 +2431,12 @@
         <v>96</v>
       </c>
       <c r="B97" s="2"/>
-      <c r="C97" s="2"/>
+      <c r="C97" s="14"/>
       <c r="D97" s="2"/>
       <c r="E97" s="5"/>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
-      <c r="H97" s="2"/>
+      <c r="H97" s="10"/>
       <c r="I97" s="2"/>
       <c r="J97" s="3"/>
       <c r="K97" s="3"/>
@@ -2402,12 +2450,12 @@
         <v>97</v>
       </c>
       <c r="B98" s="2"/>
-      <c r="C98" s="2"/>
+      <c r="C98" s="14"/>
       <c r="D98" s="2"/>
       <c r="E98" s="5"/>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
-      <c r="H98" s="2"/>
+      <c r="H98" s="10"/>
       <c r="I98" s="2"/>
       <c r="J98" s="3"/>
       <c r="K98" s="3"/>
@@ -2421,12 +2469,12 @@
         <v>98</v>
       </c>
       <c r="B99" s="2"/>
-      <c r="C99" s="2"/>
+      <c r="C99" s="14"/>
       <c r="D99" s="2"/>
       <c r="E99" s="5"/>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
-      <c r="H99" s="2"/>
+      <c r="H99" s="10"/>
       <c r="I99" s="2"/>
       <c r="J99" s="3"/>
       <c r="K99" s="3"/>
@@ -2440,12 +2488,12 @@
         <v>99</v>
       </c>
       <c r="B100" s="2"/>
-      <c r="C100" s="2"/>
+      <c r="C100" s="14"/>
       <c r="D100" s="2"/>
       <c r="E100" s="5"/>
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
-      <c r="H100" s="2"/>
+      <c r="H100" s="10"/>
       <c r="I100" s="2"/>
       <c r="J100" s="3"/>
       <c r="K100" s="3"/>
@@ -2459,12 +2507,12 @@
         <v>100</v>
       </c>
       <c r="B101" s="2"/>
-      <c r="C101" s="2"/>
+      <c r="C101" s="14"/>
       <c r="D101" s="2"/>
       <c r="E101" s="5"/>
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
-      <c r="H101" s="2"/>
+      <c r="H101" s="10"/>
       <c r="I101" s="2"/>
       <c r="J101" s="3"/>
       <c r="K101" s="3"/>
@@ -2478,12 +2526,12 @@
         <v>101</v>
       </c>
       <c r="B102" s="2"/>
-      <c r="C102" s="2"/>
+      <c r="C102" s="14"/>
       <c r="D102" s="2"/>
       <c r="E102" s="5"/>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
-      <c r="H102" s="2"/>
+      <c r="H102" s="10"/>
       <c r="I102" s="2"/>
       <c r="J102" s="3"/>
       <c r="K102" s="3"/>
@@ -2497,12 +2545,12 @@
         <v>102</v>
       </c>
       <c r="B103" s="2"/>
-      <c r="C103" s="2"/>
+      <c r="C103" s="14"/>
       <c r="D103" s="2"/>
       <c r="E103" s="5"/>
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
-      <c r="H103" s="2"/>
+      <c r="H103" s="10"/>
       <c r="I103" s="2"/>
       <c r="J103" s="3"/>
       <c r="K103" s="3"/>
@@ -2516,12 +2564,12 @@
         <v>103</v>
       </c>
       <c r="B104" s="2"/>
-      <c r="C104" s="2"/>
+      <c r="C104" s="14"/>
       <c r="D104" s="2"/>
       <c r="E104" s="5"/>
       <c r="F104" s="2"/>
       <c r="G104" s="2"/>
-      <c r="H104" s="2"/>
+      <c r="H104" s="10"/>
       <c r="I104" s="2"/>
       <c r="J104" s="3"/>
       <c r="K104" s="3"/>
@@ -2535,12 +2583,12 @@
         <v>104</v>
       </c>
       <c r="B105" s="2"/>
-      <c r="C105" s="2"/>
+      <c r="C105" s="14"/>
       <c r="D105" s="2"/>
       <c r="E105" s="5"/>
       <c r="F105" s="2"/>
       <c r="G105" s="2"/>
-      <c r="H105" s="2"/>
+      <c r="H105" s="10"/>
       <c r="I105" s="2"/>
       <c r="J105" s="3"/>
       <c r="K105" s="3"/>
@@ -2554,12 +2602,12 @@
         <v>105</v>
       </c>
       <c r="B106" s="2"/>
-      <c r="C106" s="2"/>
+      <c r="C106" s="14"/>
       <c r="D106" s="2"/>
       <c r="E106" s="5"/>
       <c r="F106" s="2"/>
       <c r="G106" s="2"/>
-      <c r="H106" s="2"/>
+      <c r="H106" s="10"/>
       <c r="I106" s="2"/>
       <c r="J106" s="3"/>
       <c r="K106" s="3"/>
@@ -2573,12 +2621,12 @@
         <v>106</v>
       </c>
       <c r="B107" s="2"/>
-      <c r="C107" s="2"/>
+      <c r="C107" s="14"/>
       <c r="D107" s="2"/>
       <c r="E107" s="5"/>
       <c r="F107" s="2"/>
       <c r="G107" s="2"/>
-      <c r="H107" s="2"/>
+      <c r="H107" s="10"/>
       <c r="I107" s="2"/>
       <c r="J107" s="3"/>
       <c r="K107" s="3"/>
@@ -2592,12 +2640,12 @@
         <v>107</v>
       </c>
       <c r="B108" s="2"/>
-      <c r="C108" s="2"/>
+      <c r="C108" s="14"/>
       <c r="D108" s="2"/>
       <c r="E108" s="5"/>
       <c r="F108" s="2"/>
       <c r="G108" s="2"/>
-      <c r="H108" s="2"/>
+      <c r="H108" s="10"/>
       <c r="I108" s="2"/>
       <c r="J108" s="3"/>
       <c r="K108" s="3"/>
@@ -2611,12 +2659,12 @@
         <v>108</v>
       </c>
       <c r="B109" s="2"/>
-      <c r="C109" s="2"/>
+      <c r="C109" s="14"/>
       <c r="D109" s="2"/>
       <c r="E109" s="5"/>
       <c r="F109" s="2"/>
       <c r="G109" s="2"/>
-      <c r="H109" s="2"/>
+      <c r="H109" s="10"/>
       <c r="I109" s="2"/>
       <c r="J109" s="3"/>
       <c r="K109" s="3"/>
@@ -2630,12 +2678,12 @@
         <v>109</v>
       </c>
       <c r="B110" s="2"/>
-      <c r="C110" s="2"/>
+      <c r="C110" s="14"/>
       <c r="D110" s="2"/>
       <c r="E110" s="5"/>
       <c r="F110" s="2"/>
       <c r="G110" s="2"/>
-      <c r="H110" s="2"/>
+      <c r="H110" s="10"/>
       <c r="I110" s="2"/>
       <c r="J110" s="3"/>
       <c r="K110" s="3"/>
@@ -2649,12 +2697,12 @@
         <v>110</v>
       </c>
       <c r="B111" s="2"/>
-      <c r="C111" s="2"/>
+      <c r="C111" s="14"/>
       <c r="D111" s="2"/>
       <c r="E111" s="5"/>
       <c r="F111" s="2"/>
       <c r="G111" s="2"/>
-      <c r="H111" s="2"/>
+      <c r="H111" s="10"/>
       <c r="I111" s="2"/>
       <c r="J111" s="3"/>
       <c r="K111" s="3"/>
@@ -2668,12 +2716,12 @@
         <v>111</v>
       </c>
       <c r="B112" s="2"/>
-      <c r="C112" s="2"/>
+      <c r="C112" s="14"/>
       <c r="D112" s="2"/>
       <c r="E112" s="5"/>
       <c r="F112" s="2"/>
       <c r="G112" s="2"/>
-      <c r="H112" s="2"/>
+      <c r="H112" s="10"/>
       <c r="I112" s="2"/>
       <c r="J112" s="3"/>
       <c r="K112" s="3"/>
@@ -2687,12 +2735,12 @@
         <v>112</v>
       </c>
       <c r="B113" s="2"/>
-      <c r="C113" s="2"/>
+      <c r="C113" s="14"/>
       <c r="D113" s="2"/>
       <c r="E113" s="5"/>
       <c r="F113" s="2"/>
       <c r="G113" s="2"/>
-      <c r="H113" s="2"/>
+      <c r="H113" s="10"/>
       <c r="I113" s="2"/>
       <c r="J113" s="3"/>
       <c r="K113" s="3"/>
@@ -2706,12 +2754,12 @@
         <v>113</v>
       </c>
       <c r="B114" s="2"/>
-      <c r="C114" s="2"/>
+      <c r="C114" s="14"/>
       <c r="D114" s="2"/>
       <c r="E114" s="5"/>
       <c r="F114" s="2"/>
       <c r="G114" s="2"/>
-      <c r="H114" s="2"/>
+      <c r="H114" s="10"/>
       <c r="I114" s="2"/>
       <c r="J114" s="3"/>
       <c r="K114" s="3"/>
@@ -2725,12 +2773,12 @@
         <v>114</v>
       </c>
       <c r="B115" s="2"/>
-      <c r="C115" s="2"/>
+      <c r="C115" s="14"/>
       <c r="D115" s="2"/>
       <c r="E115" s="5"/>
       <c r="F115" s="2"/>
       <c r="G115" s="2"/>
-      <c r="H115" s="2"/>
+      <c r="H115" s="10"/>
       <c r="I115" s="2"/>
       <c r="J115" s="3"/>
       <c r="K115" s="3"/>
@@ -2744,12 +2792,12 @@
         <v>115</v>
       </c>
       <c r="B116" s="2"/>
-      <c r="C116" s="2"/>
+      <c r="C116" s="14"/>
       <c r="D116" s="2"/>
       <c r="E116" s="5"/>
       <c r="F116" s="2"/>
       <c r="G116" s="2"/>
-      <c r="H116" s="2"/>
+      <c r="H116" s="10"/>
       <c r="I116" s="2"/>
       <c r="J116" s="3"/>
       <c r="K116" s="3"/>
@@ -2763,12 +2811,12 @@
         <v>116</v>
       </c>
       <c r="B117" s="2"/>
-      <c r="C117" s="2"/>
+      <c r="C117" s="14"/>
       <c r="D117" s="2"/>
       <c r="E117" s="5"/>
       <c r="F117" s="2"/>
       <c r="G117" s="2"/>
-      <c r="H117" s="2"/>
+      <c r="H117" s="10"/>
       <c r="I117" s="2"/>
       <c r="J117" s="3"/>
       <c r="K117" s="3"/>
@@ -2782,12 +2830,12 @@
         <v>117</v>
       </c>
       <c r="B118" s="2"/>
-      <c r="C118" s="2"/>
+      <c r="C118" s="14"/>
       <c r="D118" s="2"/>
       <c r="E118" s="5"/>
       <c r="F118" s="2"/>
       <c r="G118" s="2"/>
-      <c r="H118" s="2"/>
+      <c r="H118" s="10"/>
       <c r="I118" s="2"/>
       <c r="J118" s="3"/>
       <c r="K118" s="3"/>
@@ -2801,12 +2849,12 @@
         <v>118</v>
       </c>
       <c r="B119" s="2"/>
-      <c r="C119" s="2"/>
+      <c r="C119" s="14"/>
       <c r="D119" s="2"/>
       <c r="E119" s="5"/>
       <c r="F119" s="2"/>
       <c r="G119" s="2"/>
-      <c r="H119" s="2"/>
+      <c r="H119" s="10"/>
       <c r="I119" s="2"/>
       <c r="J119" s="3"/>
       <c r="K119" s="3"/>
@@ -2820,12 +2868,12 @@
         <v>119</v>
       </c>
       <c r="B120" s="2"/>
-      <c r="C120" s="2"/>
+      <c r="C120" s="14"/>
       <c r="D120" s="2"/>
       <c r="E120" s="5"/>
       <c r="F120" s="2"/>
       <c r="G120" s="2"/>
-      <c r="H120" s="2"/>
+      <c r="H120" s="10"/>
       <c r="I120" s="2"/>
       <c r="J120" s="3"/>
       <c r="K120" s="3"/>
@@ -2839,12 +2887,12 @@
         <v>120</v>
       </c>
       <c r="B121" s="2"/>
-      <c r="C121" s="2"/>
+      <c r="C121" s="14"/>
       <c r="D121" s="2"/>
       <c r="E121" s="5"/>
       <c r="F121" s="2"/>
       <c r="G121" s="2"/>
-      <c r="H121" s="2"/>
+      <c r="H121" s="10"/>
       <c r="I121" s="2"/>
       <c r="J121" s="3"/>
       <c r="K121" s="3"/>
@@ -2858,12 +2906,12 @@
         <v>121</v>
       </c>
       <c r="B122" s="2"/>
-      <c r="C122" s="2"/>
+      <c r="C122" s="14"/>
       <c r="D122" s="2"/>
       <c r="E122" s="5"/>
       <c r="F122" s="2"/>
       <c r="G122" s="2"/>
-      <c r="H122" s="2"/>
+      <c r="H122" s="10"/>
       <c r="I122" s="2"/>
       <c r="J122" s="3"/>
       <c r="K122" s="3"/>
@@ -2877,12 +2925,12 @@
         <v>122</v>
       </c>
       <c r="B123" s="2"/>
-      <c r="C123" s="2"/>
+      <c r="C123" s="14"/>
       <c r="D123" s="2"/>
       <c r="E123" s="5"/>
       <c r="F123" s="2"/>
       <c r="G123" s="2"/>
-      <c r="H123" s="2"/>
+      <c r="H123" s="10"/>
       <c r="I123" s="2"/>
       <c r="J123" s="3"/>
       <c r="K123" s="3"/>
@@ -2896,12 +2944,12 @@
         <v>123</v>
       </c>
       <c r="B124" s="2"/>
-      <c r="C124" s="2"/>
+      <c r="C124" s="14"/>
       <c r="D124" s="2"/>
       <c r="E124" s="5"/>
       <c r="F124" s="2"/>
       <c r="G124" s="2"/>
-      <c r="H124" s="2"/>
+      <c r="H124" s="10"/>
       <c r="I124" s="2"/>
       <c r="J124" s="3"/>
       <c r="K124" s="3"/>
@@ -2915,12 +2963,12 @@
         <v>124</v>
       </c>
       <c r="B125" s="2"/>
-      <c r="C125" s="2"/>
+      <c r="C125" s="14"/>
       <c r="D125" s="2"/>
       <c r="E125" s="5"/>
       <c r="F125" s="2"/>
       <c r="G125" s="2"/>
-      <c r="H125" s="2"/>
+      <c r="H125" s="10"/>
       <c r="I125" s="2"/>
       <c r="J125" s="3"/>
       <c r="K125" s="3"/>
@@ -2934,12 +2982,12 @@
         <v>125</v>
       </c>
       <c r="B126" s="2"/>
-      <c r="C126" s="2"/>
+      <c r="C126" s="14"/>
       <c r="D126" s="2"/>
       <c r="E126" s="5"/>
       <c r="F126" s="2"/>
       <c r="G126" s="2"/>
-      <c r="H126" s="2"/>
+      <c r="H126" s="10"/>
       <c r="I126" s="2"/>
       <c r="J126" s="3"/>
       <c r="K126" s="3"/>
@@ -2953,12 +3001,12 @@
         <v>126</v>
       </c>
       <c r="B127" s="2"/>
-      <c r="C127" s="2"/>
+      <c r="C127" s="14"/>
       <c r="D127" s="2"/>
       <c r="E127" s="5"/>
       <c r="F127" s="2"/>
       <c r="G127" s="2"/>
-      <c r="H127" s="2"/>
+      <c r="H127" s="10"/>
       <c r="I127" s="2"/>
       <c r="J127" s="3"/>
       <c r="K127" s="3"/>
@@ -2972,12 +3020,12 @@
         <v>127</v>
       </c>
       <c r="B128" s="2"/>
-      <c r="C128" s="2"/>
+      <c r="C128" s="14"/>
       <c r="D128" s="2"/>
       <c r="E128" s="5"/>
       <c r="F128" s="2"/>
       <c r="G128" s="2"/>
-      <c r="H128" s="2"/>
+      <c r="H128" s="10"/>
       <c r="I128" s="2"/>
       <c r="J128" s="3"/>
       <c r="K128" s="3"/>
@@ -2991,12 +3039,12 @@
         <v>128</v>
       </c>
       <c r="B129" s="2"/>
-      <c r="C129" s="2"/>
+      <c r="C129" s="14"/>
       <c r="D129" s="2"/>
       <c r="E129" s="5"/>
       <c r="F129" s="2"/>
       <c r="G129" s="2"/>
-      <c r="H129" s="2"/>
+      <c r="H129" s="10"/>
       <c r="I129" s="2"/>
       <c r="J129" s="3"/>
       <c r="K129" s="3"/>
@@ -3010,12 +3058,12 @@
         <v>129</v>
       </c>
       <c r="B130" s="2"/>
-      <c r="C130" s="2"/>
+      <c r="C130" s="14"/>
       <c r="D130" s="2"/>
       <c r="E130" s="5"/>
       <c r="F130" s="2"/>
       <c r="G130" s="2"/>
-      <c r="H130" s="2"/>
+      <c r="H130" s="10"/>
       <c r="I130" s="2"/>
       <c r="J130" s="3"/>
       <c r="K130" s="3"/>
@@ -3029,12 +3077,12 @@
         <v>130</v>
       </c>
       <c r="B131" s="2"/>
-      <c r="C131" s="2"/>
+      <c r="C131" s="14"/>
       <c r="D131" s="2"/>
       <c r="E131" s="5"/>
       <c r="F131" s="2"/>
       <c r="G131" s="2"/>
-      <c r="H131" s="2"/>
+      <c r="H131" s="10"/>
       <c r="I131" s="2"/>
       <c r="J131" s="3"/>
       <c r="K131" s="3"/>
@@ -3048,12 +3096,12 @@
         <v>131</v>
       </c>
       <c r="B132" s="2"/>
-      <c r="C132" s="2"/>
+      <c r="C132" s="14"/>
       <c r="D132" s="2"/>
       <c r="E132" s="5"/>
       <c r="F132" s="2"/>
       <c r="G132" s="2"/>
-      <c r="H132" s="2"/>
+      <c r="H132" s="10"/>
       <c r="I132" s="2"/>
       <c r="J132" s="3"/>
       <c r="K132" s="3"/>
@@ -3067,12 +3115,12 @@
         <v>132</v>
       </c>
       <c r="B133" s="2"/>
-      <c r="C133" s="2"/>
+      <c r="C133" s="14"/>
       <c r="D133" s="2"/>
       <c r="E133" s="5"/>
       <c r="F133" s="2"/>
       <c r="G133" s="2"/>
-      <c r="H133" s="2"/>
+      <c r="H133" s="10"/>
       <c r="I133" s="2"/>
       <c r="J133" s="3"/>
       <c r="K133" s="3"/>
@@ -3086,12 +3134,12 @@
         <v>133</v>
       </c>
       <c r="B134" s="2"/>
-      <c r="C134" s="2"/>
+      <c r="C134" s="14"/>
       <c r="D134" s="2"/>
       <c r="E134" s="5"/>
       <c r="F134" s="2"/>
       <c r="G134" s="2"/>
-      <c r="H134" s="2"/>
+      <c r="H134" s="10"/>
       <c r="I134" s="2"/>
       <c r="J134" s="3"/>
       <c r="K134" s="3"/>
@@ -3105,12 +3153,12 @@
         <v>134</v>
       </c>
       <c r="B135" s="2"/>
-      <c r="C135" s="2"/>
+      <c r="C135" s="14"/>
       <c r="D135" s="2"/>
       <c r="E135" s="5"/>
       <c r="F135" s="2"/>
       <c r="G135" s="2"/>
-      <c r="H135" s="2"/>
+      <c r="H135" s="10"/>
       <c r="I135" s="2"/>
       <c r="J135" s="3"/>
       <c r="K135" s="3"/>
@@ -3124,12 +3172,12 @@
         <v>135</v>
       </c>
       <c r="B136" s="2"/>
-      <c r="C136" s="2"/>
+      <c r="C136" s="14"/>
       <c r="D136" s="2"/>
       <c r="E136" s="5"/>
       <c r="F136" s="2"/>
       <c r="G136" s="2"/>
-      <c r="H136" s="2"/>
+      <c r="H136" s="10"/>
       <c r="I136" s="2"/>
       <c r="J136" s="3"/>
       <c r="K136" s="3"/>
@@ -3143,12 +3191,12 @@
         <v>136</v>
       </c>
       <c r="B137" s="2"/>
-      <c r="C137" s="2"/>
+      <c r="C137" s="14"/>
       <c r="D137" s="2"/>
       <c r="E137" s="5"/>
       <c r="F137" s="2"/>
       <c r="G137" s="2"/>
-      <c r="H137" s="2"/>
+      <c r="H137" s="10"/>
       <c r="I137" s="2"/>
       <c r="J137" s="3"/>
       <c r="K137" s="3"/>
@@ -3162,12 +3210,12 @@
         <v>137</v>
       </c>
       <c r="B138" s="2"/>
-      <c r="C138" s="2"/>
+      <c r="C138" s="14"/>
       <c r="D138" s="2"/>
       <c r="E138" s="5"/>
       <c r="F138" s="2"/>
       <c r="G138" s="2"/>
-      <c r="H138" s="2"/>
+      <c r="H138" s="10"/>
       <c r="I138" s="2"/>
       <c r="J138" s="3"/>
       <c r="K138" s="3"/>
@@ -3181,12 +3229,12 @@
         <v>138</v>
       </c>
       <c r="B139" s="2"/>
-      <c r="C139" s="2"/>
+      <c r="C139" s="14"/>
       <c r="D139" s="2"/>
       <c r="E139" s="5"/>
       <c r="F139" s="2"/>
       <c r="G139" s="2"/>
-      <c r="H139" s="2"/>
+      <c r="H139" s="10"/>
       <c r="I139" s="2"/>
       <c r="J139" s="3"/>
       <c r="K139" s="3"/>
@@ -3200,12 +3248,12 @@
         <v>139</v>
       </c>
       <c r="B140" s="2"/>
-      <c r="C140" s="2"/>
+      <c r="C140" s="14"/>
       <c r="D140" s="2"/>
       <c r="E140" s="5"/>
       <c r="F140" s="2"/>
       <c r="G140" s="2"/>
-      <c r="H140" s="2"/>
+      <c r="H140" s="10"/>
       <c r="I140" s="2"/>
       <c r="J140" s="3"/>
       <c r="K140" s="3"/>
@@ -3219,12 +3267,12 @@
         <v>140</v>
       </c>
       <c r="B141" s="2"/>
-      <c r="C141" s="2"/>
+      <c r="C141" s="14"/>
       <c r="D141" s="2"/>
       <c r="E141" s="5"/>
       <c r="F141" s="2"/>
       <c r="G141" s="2"/>
-      <c r="H141" s="2"/>
+      <c r="H141" s="10"/>
       <c r="I141" s="2"/>
       <c r="J141" s="3"/>
       <c r="K141" s="3"/>
@@ -3238,12 +3286,12 @@
         <v>141</v>
       </c>
       <c r="B142" s="2"/>
-      <c r="C142" s="2"/>
+      <c r="C142" s="14"/>
       <c r="D142" s="2"/>
       <c r="E142" s="5"/>
       <c r="F142" s="2"/>
       <c r="G142" s="2"/>
-      <c r="H142" s="2"/>
+      <c r="H142" s="10"/>
       <c r="I142" s="2"/>
       <c r="J142" s="3"/>
       <c r="K142" s="3"/>
@@ -3257,12 +3305,12 @@
         <v>142</v>
       </c>
       <c r="B143" s="2"/>
-      <c r="C143" s="2"/>
+      <c r="C143" s="14"/>
       <c r="D143" s="2"/>
       <c r="E143" s="5"/>
       <c r="F143" s="2"/>
       <c r="G143" s="2"/>
-      <c r="H143" s="2"/>
+      <c r="H143" s="10"/>
       <c r="I143" s="2"/>
       <c r="J143" s="3"/>
       <c r="K143" s="3"/>
@@ -3276,12 +3324,12 @@
         <v>143</v>
       </c>
       <c r="B144" s="2"/>
-      <c r="C144" s="2"/>
+      <c r="C144" s="14"/>
       <c r="D144" s="2"/>
       <c r="E144" s="5"/>
       <c r="F144" s="2"/>
       <c r="G144" s="2"/>
-      <c r="H144" s="2"/>
+      <c r="H144" s="10"/>
       <c r="I144" s="2"/>
       <c r="J144" s="3"/>
       <c r="K144" s="3"/>
@@ -3295,12 +3343,12 @@
         <v>144</v>
       </c>
       <c r="B145" s="2"/>
-      <c r="C145" s="2"/>
+      <c r="C145" s="14"/>
       <c r="D145" s="2"/>
       <c r="E145" s="5"/>
       <c r="F145" s="2"/>
       <c r="G145" s="2"/>
-      <c r="H145" s="2"/>
+      <c r="H145" s="10"/>
       <c r="I145" s="2"/>
       <c r="J145" s="3"/>
       <c r="K145" s="3"/>
@@ -3314,12 +3362,12 @@
         <v>145</v>
       </c>
       <c r="B146" s="2"/>
-      <c r="C146" s="2"/>
+      <c r="C146" s="14"/>
       <c r="D146" s="2"/>
       <c r="E146" s="5"/>
       <c r="F146" s="2"/>
       <c r="G146" s="2"/>
-      <c r="H146" s="2"/>
+      <c r="H146" s="10"/>
       <c r="I146" s="2"/>
       <c r="J146" s="3"/>
       <c r="K146" s="3"/>
@@ -3333,12 +3381,12 @@
         <v>146</v>
       </c>
       <c r="B147" s="2"/>
-      <c r="C147" s="2"/>
+      <c r="C147" s="14"/>
       <c r="D147" s="2"/>
       <c r="E147" s="5"/>
       <c r="F147" s="2"/>
       <c r="G147" s="2"/>
-      <c r="H147" s="2"/>
+      <c r="H147" s="10"/>
       <c r="I147" s="2"/>
       <c r="J147" s="3"/>
       <c r="K147" s="3"/>
@@ -3352,12 +3400,12 @@
         <v>147</v>
       </c>
       <c r="B148" s="2"/>
-      <c r="C148" s="2"/>
+      <c r="C148" s="14"/>
       <c r="D148" s="2"/>
       <c r="E148" s="5"/>
       <c r="F148" s="2"/>
       <c r="G148" s="2"/>
-      <c r="H148" s="2"/>
+      <c r="H148" s="10"/>
       <c r="I148" s="2"/>
       <c r="J148" s="3"/>
       <c r="K148" s="3"/>
@@ -3371,12 +3419,12 @@
         <v>148</v>
       </c>
       <c r="B149" s="2"/>
-      <c r="C149" s="2"/>
+      <c r="C149" s="14"/>
       <c r="D149" s="2"/>
       <c r="E149" s="5"/>
       <c r="F149" s="2"/>
       <c r="G149" s="2"/>
-      <c r="H149" s="2"/>
+      <c r="H149" s="10"/>
       <c r="I149" s="2"/>
       <c r="J149" s="3"/>
       <c r="K149" s="3"/>
@@ -3390,12 +3438,12 @@
         <v>149</v>
       </c>
       <c r="B150" s="2"/>
-      <c r="C150" s="2"/>
+      <c r="C150" s="14"/>
       <c r="D150" s="2"/>
       <c r="E150" s="5"/>
       <c r="F150" s="2"/>
       <c r="G150" s="2"/>
-      <c r="H150" s="2"/>
+      <c r="H150" s="10"/>
       <c r="I150" s="2"/>
       <c r="J150" s="3"/>
       <c r="K150" s="3"/>
@@ -3409,12 +3457,12 @@
         <v>150</v>
       </c>
       <c r="B151" s="2"/>
-      <c r="C151" s="2"/>
+      <c r="C151" s="14"/>
       <c r="D151" s="2"/>
       <c r="E151" s="5"/>
       <c r="F151" s="2"/>
       <c r="G151" s="2"/>
-      <c r="H151" s="2"/>
+      <c r="H151" s="10"/>
       <c r="I151" s="2"/>
       <c r="J151" s="3"/>
       <c r="K151" s="3"/>
@@ -3426,12 +3474,12 @@
     <row r="152" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A152" s="3"/>
       <c r="B152" s="3"/>
-      <c r="C152" s="3"/>
+      <c r="C152" s="16"/>
       <c r="D152" s="3"/>
       <c r="E152" s="6"/>
       <c r="F152" s="3"/>
       <c r="G152" s="3"/>
-      <c r="H152" s="3"/>
+      <c r="H152" s="12"/>
       <c r="I152" s="3"/>
       <c r="J152" s="3"/>
       <c r="K152" s="3"/>
@@ -3443,12 +3491,12 @@
     <row r="153" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A153" s="3"/>
       <c r="B153" s="3"/>
-      <c r="C153" s="3"/>
+      <c r="C153" s="16"/>
       <c r="D153" s="3"/>
       <c r="E153" s="6"/>
       <c r="F153" s="3"/>
       <c r="G153" s="3"/>
-      <c r="H153" s="3"/>
+      <c r="H153" s="12"/>
       <c r="I153" s="3"/>
       <c r="J153" s="3"/>
       <c r="K153" s="3"/>
@@ -3460,12 +3508,12 @@
     <row r="154" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A154" s="3"/>
       <c r="B154" s="3"/>
-      <c r="C154" s="3"/>
+      <c r="C154" s="16"/>
       <c r="D154" s="3"/>
       <c r="E154" s="6"/>
       <c r="F154" s="3"/>
       <c r="G154" s="3"/>
-      <c r="H154" s="3"/>
+      <c r="H154" s="12"/>
       <c r="I154" s="3"/>
       <c r="J154" s="3"/>
       <c r="K154" s="3"/>
@@ -3477,12 +3525,12 @@
     <row r="155" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A155" s="3"/>
       <c r="B155" s="3"/>
-      <c r="C155" s="3"/>
+      <c r="C155" s="16"/>
       <c r="D155" s="3"/>
       <c r="E155" s="6"/>
       <c r="F155" s="3"/>
       <c r="G155" s="3"/>
-      <c r="H155" s="3"/>
+      <c r="H155" s="12"/>
       <c r="I155" s="3"/>
       <c r="J155" s="3"/>
       <c r="K155" s="3"/>
@@ -3494,12 +3542,12 @@
     <row r="156" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A156" s="3"/>
       <c r="B156" s="3"/>
-      <c r="C156" s="3"/>
+      <c r="C156" s="16"/>
       <c r="D156" s="3"/>
       <c r="E156" s="6"/>
       <c r="F156" s="3"/>
       <c r="G156" s="3"/>
-      <c r="H156" s="3"/>
+      <c r="H156" s="12"/>
       <c r="I156" s="3"/>
       <c r="J156" s="3"/>
       <c r="K156" s="3"/>
@@ -3511,12 +3559,12 @@
     <row r="157" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A157" s="3"/>
       <c r="B157" s="3"/>
-      <c r="C157" s="3"/>
+      <c r="C157" s="16"/>
       <c r="D157" s="3"/>
       <c r="E157" s="6"/>
       <c r="F157" s="3"/>
       <c r="G157" s="3"/>
-      <c r="H157" s="3"/>
+      <c r="H157" s="12"/>
       <c r="I157" s="3"/>
       <c r="J157" s="3"/>
       <c r="K157" s="3"/>
@@ -3528,12 +3576,12 @@
     <row r="158" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A158" s="3"/>
       <c r="B158" s="3"/>
-      <c r="C158" s="3"/>
+      <c r="C158" s="16"/>
       <c r="D158" s="3"/>
       <c r="E158" s="6"/>
       <c r="F158" s="3"/>
       <c r="G158" s="3"/>
-      <c r="H158" s="3"/>
+      <c r="H158" s="12"/>
       <c r="I158" s="3"/>
       <c r="J158" s="3"/>
       <c r="K158" s="3"/>
@@ -3545,12 +3593,12 @@
     <row r="159" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A159" s="3"/>
       <c r="B159" s="3"/>
-      <c r="C159" s="3"/>
+      <c r="C159" s="16"/>
       <c r="D159" s="3"/>
       <c r="E159" s="6"/>
       <c r="F159" s="3"/>
       <c r="G159" s="3"/>
-      <c r="H159" s="3"/>
+      <c r="H159" s="12"/>
       <c r="I159" s="3"/>
       <c r="J159" s="3"/>
       <c r="K159" s="3"/>
@@ -3562,12 +3610,12 @@
     <row r="160" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A160" s="3"/>
       <c r="B160" s="3"/>
-      <c r="C160" s="3"/>
+      <c r="C160" s="16"/>
       <c r="D160" s="3"/>
       <c r="E160" s="6"/>
       <c r="F160" s="3"/>
       <c r="G160" s="3"/>
-      <c r="H160" s="3"/>
+      <c r="H160" s="12"/>
       <c r="I160" s="3"/>
       <c r="J160" s="3"/>
       <c r="K160" s="3"/>
@@ -3579,12 +3627,12 @@
     <row r="161" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A161" s="3"/>
       <c r="B161" s="3"/>
-      <c r="C161" s="3"/>
+      <c r="C161" s="16"/>
       <c r="D161" s="3"/>
       <c r="E161" s="6"/>
       <c r="F161" s="3"/>
       <c r="G161" s="3"/>
-      <c r="H161" s="3"/>
+      <c r="H161" s="12"/>
       <c r="I161" s="3"/>
       <c r="J161" s="3"/>
       <c r="K161" s="3"/>
@@ -3596,12 +3644,12 @@
     <row r="162" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A162" s="3"/>
       <c r="B162" s="3"/>
-      <c r="C162" s="3"/>
+      <c r="C162" s="16"/>
       <c r="D162" s="3"/>
       <c r="E162" s="6"/>
       <c r="F162" s="3"/>
       <c r="G162" s="3"/>
-      <c r="H162" s="3"/>
+      <c r="H162" s="12"/>
       <c r="I162" s="3"/>
       <c r="J162" s="3"/>
       <c r="K162" s="3"/>
@@ -3613,12 +3661,12 @@
     <row r="163" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A163" s="3"/>
       <c r="B163" s="3"/>
-      <c r="C163" s="3"/>
+      <c r="C163" s="16"/>
       <c r="D163" s="3"/>
       <c r="E163" s="6"/>
       <c r="F163" s="3"/>
       <c r="G163" s="3"/>
-      <c r="H163" s="3"/>
+      <c r="H163" s="12"/>
       <c r="I163" s="3"/>
       <c r="J163" s="3"/>
       <c r="K163" s="3"/>
@@ -3630,12 +3678,12 @@
     <row r="164" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A164" s="3"/>
       <c r="B164" s="3"/>
-      <c r="C164" s="3"/>
+      <c r="C164" s="16"/>
       <c r="D164" s="3"/>
       <c r="E164" s="6"/>
       <c r="F164" s="3"/>
       <c r="G164" s="3"/>
-      <c r="H164" s="3"/>
+      <c r="H164" s="12"/>
       <c r="I164" s="3"/>
       <c r="J164" s="3"/>
       <c r="K164" s="3"/>
@@ -3647,12 +3695,12 @@
     <row r="165" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A165" s="3"/>
       <c r="B165" s="3"/>
-      <c r="C165" s="3"/>
+      <c r="C165" s="16"/>
       <c r="D165" s="3"/>
       <c r="E165" s="6"/>
       <c r="F165" s="3"/>
       <c r="G165" s="3"/>
-      <c r="H165" s="3"/>
+      <c r="H165" s="12"/>
       <c r="I165" s="3"/>
       <c r="J165" s="3"/>
       <c r="K165" s="3"/>
@@ -3664,12 +3712,12 @@
     <row r="166" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A166" s="3"/>
       <c r="B166" s="3"/>
-      <c r="C166" s="3"/>
+      <c r="C166" s="16"/>
       <c r="D166" s="3"/>
       <c r="E166" s="6"/>
       <c r="F166" s="3"/>
       <c r="G166" s="3"/>
-      <c r="H166" s="3"/>
+      <c r="H166" s="12"/>
       <c r="I166" s="3"/>
       <c r="J166" s="3"/>
       <c r="K166" s="3"/>
@@ -3681,12 +3729,12 @@
     <row r="167" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A167" s="3"/>
       <c r="B167" s="3"/>
-      <c r="C167" s="3"/>
+      <c r="C167" s="16"/>
       <c r="D167" s="3"/>
       <c r="E167" s="6"/>
       <c r="F167" s="3"/>
       <c r="G167" s="3"/>
-      <c r="H167" s="3"/>
+      <c r="H167" s="12"/>
       <c r="I167" s="3"/>
       <c r="J167" s="3"/>
       <c r="K167" s="3"/>
@@ -3698,12 +3746,12 @@
     <row r="168" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A168" s="3"/>
       <c r="B168" s="3"/>
-      <c r="C168" s="3"/>
+      <c r="C168" s="16"/>
       <c r="D168" s="3"/>
       <c r="E168" s="6"/>
       <c r="F168" s="3"/>
       <c r="G168" s="3"/>
-      <c r="H168" s="3"/>
+      <c r="H168" s="12"/>
       <c r="I168" s="3"/>
       <c r="J168" s="3"/>
       <c r="K168" s="3"/>
@@ -3715,12 +3763,12 @@
     <row r="169" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A169" s="3"/>
       <c r="B169" s="3"/>
-      <c r="C169" s="3"/>
+      <c r="C169" s="16"/>
       <c r="D169" s="3"/>
       <c r="E169" s="6"/>
       <c r="F169" s="3"/>
       <c r="G169" s="3"/>
-      <c r="H169" s="3"/>
+      <c r="H169" s="12"/>
       <c r="I169" s="3"/>
       <c r="J169" s="3"/>
       <c r="K169" s="3"/>
@@ -3732,12 +3780,12 @@
     <row r="170" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A170" s="3"/>
       <c r="B170" s="3"/>
-      <c r="C170" s="3"/>
+      <c r="C170" s="16"/>
       <c r="D170" s="3"/>
       <c r="E170" s="6"/>
       <c r="F170" s="3"/>
       <c r="G170" s="3"/>
-      <c r="H170" s="3"/>
+      <c r="H170" s="12"/>
       <c r="I170" s="3"/>
       <c r="J170" s="3"/>
       <c r="K170" s="3"/>
@@ -3749,12 +3797,12 @@
     <row r="171" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A171" s="3"/>
       <c r="B171" s="3"/>
-      <c r="C171" s="3"/>
+      <c r="C171" s="16"/>
       <c r="D171" s="3"/>
       <c r="E171" s="6"/>
       <c r="F171" s="3"/>
       <c r="G171" s="3"/>
-      <c r="H171" s="3"/>
+      <c r="H171" s="12"/>
       <c r="I171" s="3"/>
       <c r="J171" s="3"/>
       <c r="K171" s="3"/>
@@ -3766,12 +3814,12 @@
     <row r="172" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A172" s="3"/>
       <c r="B172" s="3"/>
-      <c r="C172" s="3"/>
+      <c r="C172" s="16"/>
       <c r="D172" s="3"/>
       <c r="E172" s="6"/>
       <c r="F172" s="3"/>
       <c r="G172" s="3"/>
-      <c r="H172" s="3"/>
+      <c r="H172" s="12"/>
       <c r="I172" s="3"/>
       <c r="J172" s="3"/>
       <c r="K172" s="3"/>
@@ -3783,12 +3831,12 @@
     <row r="173" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A173" s="3"/>
       <c r="B173" s="3"/>
-      <c r="C173" s="3"/>
+      <c r="C173" s="16"/>
       <c r="D173" s="3"/>
       <c r="E173" s="6"/>
       <c r="F173" s="3"/>
       <c r="G173" s="3"/>
-      <c r="H173" s="3"/>
+      <c r="H173" s="12"/>
       <c r="I173" s="3"/>
       <c r="J173" s="3"/>
       <c r="K173" s="3"/>
@@ -3800,12 +3848,12 @@
     <row r="174" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A174" s="3"/>
       <c r="B174" s="3"/>
-      <c r="C174" s="3"/>
+      <c r="C174" s="16"/>
       <c r="D174" s="3"/>
       <c r="E174" s="6"/>
       <c r="F174" s="3"/>
       <c r="G174" s="3"/>
-      <c r="H174" s="3"/>
+      <c r="H174" s="12"/>
       <c r="I174" s="3"/>
       <c r="J174" s="3"/>
       <c r="K174" s="3"/>
@@ -3817,12 +3865,12 @@
     <row r="175" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A175" s="3"/>
       <c r="B175" s="3"/>
-      <c r="C175" s="3"/>
+      <c r="C175" s="16"/>
       <c r="D175" s="3"/>
       <c r="E175" s="6"/>
       <c r="F175" s="3"/>
       <c r="G175" s="3"/>
-      <c r="H175" s="3"/>
+      <c r="H175" s="12"/>
       <c r="I175" s="3"/>
       <c r="J175" s="3"/>
       <c r="K175" s="3"/>
@@ -3834,12 +3882,12 @@
     <row r="176" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A176" s="3"/>
       <c r="B176" s="3"/>
-      <c r="C176" s="3"/>
+      <c r="C176" s="16"/>
       <c r="D176" s="3"/>
       <c r="E176" s="6"/>
       <c r="F176" s="3"/>
       <c r="G176" s="3"/>
-      <c r="H176" s="3"/>
+      <c r="H176" s="12"/>
       <c r="I176" s="3"/>
       <c r="J176" s="3"/>
       <c r="K176" s="3"/>
@@ -3851,12 +3899,12 @@
     <row r="177" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A177" s="3"/>
       <c r="B177" s="3"/>
-      <c r="C177" s="3"/>
+      <c r="C177" s="16"/>
       <c r="D177" s="3"/>
       <c r="E177" s="6"/>
       <c r="F177" s="3"/>
       <c r="G177" s="3"/>
-      <c r="H177" s="3"/>
+      <c r="H177" s="12"/>
       <c r="I177" s="3"/>
       <c r="J177" s="3"/>
       <c r="K177" s="3"/>
@@ -3868,12 +3916,12 @@
     <row r="178" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A178" s="3"/>
       <c r="B178" s="3"/>
-      <c r="C178" s="3"/>
+      <c r="C178" s="16"/>
       <c r="D178" s="3"/>
       <c r="E178" s="6"/>
       <c r="F178" s="3"/>
       <c r="G178" s="3"/>
-      <c r="H178" s="3"/>
+      <c r="H178" s="12"/>
       <c r="I178" s="3"/>
       <c r="J178" s="3"/>
       <c r="K178" s="3"/>
@@ -3885,12 +3933,12 @@
     <row r="179" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A179" s="3"/>
       <c r="B179" s="3"/>
-      <c r="C179" s="3"/>
+      <c r="C179" s="16"/>
       <c r="D179" s="3"/>
       <c r="E179" s="6"/>
       <c r="F179" s="3"/>
       <c r="G179" s="3"/>
-      <c r="H179" s="3"/>
+      <c r="H179" s="12"/>
       <c r="I179" s="3"/>
       <c r="J179" s="3"/>
       <c r="K179" s="3"/>
@@ -3902,12 +3950,12 @@
     <row r="180" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A180" s="3"/>
       <c r="B180" s="3"/>
-      <c r="C180" s="3"/>
+      <c r="C180" s="16"/>
       <c r="D180" s="3"/>
       <c r="E180" s="6"/>
       <c r="F180" s="3"/>
       <c r="G180" s="3"/>
-      <c r="H180" s="3"/>
+      <c r="H180" s="12"/>
       <c r="I180" s="3"/>
       <c r="J180" s="3"/>
       <c r="K180" s="3"/>
@@ -3919,12 +3967,12 @@
     <row r="181" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A181" s="3"/>
       <c r="B181" s="3"/>
-      <c r="C181" s="3"/>
+      <c r="C181" s="16"/>
       <c r="D181" s="3"/>
       <c r="E181" s="6"/>
       <c r="F181" s="3"/>
       <c r="G181" s="3"/>
-      <c r="H181" s="3"/>
+      <c r="H181" s="12"/>
       <c r="I181" s="3"/>
       <c r="J181" s="3"/>
       <c r="K181" s="3"/>
@@ -3936,12 +3984,12 @@
     <row r="182" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A182" s="3"/>
       <c r="B182" s="3"/>
-      <c r="C182" s="3"/>
+      <c r="C182" s="16"/>
       <c r="D182" s="3"/>
       <c r="E182" s="6"/>
       <c r="F182" s="3"/>
       <c r="G182" s="3"/>
-      <c r="H182" s="3"/>
+      <c r="H182" s="12"/>
       <c r="I182" s="3"/>
       <c r="J182" s="3"/>
       <c r="K182" s="3"/>
@@ -3953,12 +4001,12 @@
     <row r="183" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A183" s="3"/>
       <c r="B183" s="3"/>
-      <c r="C183" s="3"/>
+      <c r="C183" s="16"/>
       <c r="D183" s="3"/>
       <c r="E183" s="6"/>
       <c r="F183" s="3"/>
       <c r="G183" s="3"/>
-      <c r="H183" s="3"/>
+      <c r="H183" s="12"/>
       <c r="I183" s="3"/>
       <c r="J183" s="3"/>
       <c r="K183" s="3"/>
@@ -3970,12 +4018,12 @@
     <row r="184" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A184" s="3"/>
       <c r="B184" s="3"/>
-      <c r="C184" s="3"/>
+      <c r="C184" s="16"/>
       <c r="D184" s="3"/>
       <c r="E184" s="6"/>
       <c r="F184" s="3"/>
       <c r="G184" s="3"/>
-      <c r="H184" s="3"/>
+      <c r="H184" s="12"/>
       <c r="I184" s="3"/>
       <c r="J184" s="3"/>
       <c r="K184" s="3"/>
@@ -3987,12 +4035,12 @@
     <row r="185" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A185" s="3"/>
       <c r="B185" s="3"/>
-      <c r="C185" s="3"/>
+      <c r="C185" s="16"/>
       <c r="D185" s="3"/>
       <c r="E185" s="6"/>
       <c r="F185" s="3"/>
       <c r="G185" s="3"/>
-      <c r="H185" s="3"/>
+      <c r="H185" s="12"/>
       <c r="I185" s="3"/>
       <c r="J185" s="3"/>
       <c r="K185" s="3"/>
@@ -4004,12 +4052,12 @@
     <row r="186" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A186" s="3"/>
       <c r="B186" s="3"/>
-      <c r="C186" s="3"/>
+      <c r="C186" s="16"/>
       <c r="D186" s="3"/>
       <c r="E186" s="6"/>
       <c r="F186" s="3"/>
       <c r="G186" s="3"/>
-      <c r="H186" s="3"/>
+      <c r="H186" s="12"/>
       <c r="I186" s="3"/>
       <c r="J186" s="3"/>
       <c r="K186" s="3"/>
@@ -4021,12 +4069,12 @@
     <row r="187" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A187" s="3"/>
       <c r="B187" s="3"/>
-      <c r="C187" s="3"/>
+      <c r="C187" s="16"/>
       <c r="D187" s="3"/>
       <c r="E187" s="6"/>
       <c r="F187" s="3"/>
       <c r="G187" s="3"/>
-      <c r="H187" s="3"/>
+      <c r="H187" s="12"/>
       <c r="I187" s="3"/>
       <c r="J187" s="3"/>
       <c r="K187" s="3"/>
@@ -4038,12 +4086,12 @@
     <row r="188" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A188" s="3"/>
       <c r="B188" s="3"/>
-      <c r="C188" s="3"/>
+      <c r="C188" s="16"/>
       <c r="D188" s="3"/>
       <c r="E188" s="6"/>
       <c r="F188" s="3"/>
       <c r="G188" s="3"/>
-      <c r="H188" s="3"/>
+      <c r="H188" s="12"/>
       <c r="I188" s="3"/>
       <c r="J188" s="3"/>
       <c r="K188" s="3"/>
@@ -4055,12 +4103,12 @@
     <row r="189" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A189" s="3"/>
       <c r="B189" s="3"/>
-      <c r="C189" s="3"/>
+      <c r="C189" s="16"/>
       <c r="D189" s="3"/>
       <c r="E189" s="6"/>
       <c r="F189" s="3"/>
       <c r="G189" s="3"/>
-      <c r="H189" s="3"/>
+      <c r="H189" s="12"/>
       <c r="I189" s="3"/>
       <c r="J189" s="3"/>
       <c r="K189" s="3"/>
@@ -4072,12 +4120,12 @@
     <row r="190" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A190" s="3"/>
       <c r="B190" s="3"/>
-      <c r="C190" s="3"/>
+      <c r="C190" s="16"/>
       <c r="D190" s="3"/>
       <c r="E190" s="6"/>
       <c r="F190" s="3"/>
       <c r="G190" s="3"/>
-      <c r="H190" s="3"/>
+      <c r="H190" s="12"/>
       <c r="I190" s="3"/>
       <c r="J190" s="3"/>
       <c r="K190" s="3"/>
@@ -4089,12 +4137,12 @@
     <row r="191" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A191" s="3"/>
       <c r="B191" s="3"/>
-      <c r="C191" s="3"/>
+      <c r="C191" s="16"/>
       <c r="D191" s="3"/>
       <c r="E191" s="6"/>
       <c r="F191" s="3"/>
       <c r="G191" s="3"/>
-      <c r="H191" s="3"/>
+      <c r="H191" s="12"/>
       <c r="I191" s="3"/>
       <c r="J191" s="3"/>
       <c r="K191" s="3"/>
@@ -4106,12 +4154,12 @@
     <row r="192" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A192" s="3"/>
       <c r="B192" s="3"/>
-      <c r="C192" s="3"/>
+      <c r="C192" s="16"/>
       <c r="D192" s="3"/>
       <c r="E192" s="6"/>
       <c r="F192" s="3"/>
       <c r="G192" s="3"/>
-      <c r="H192" s="3"/>
+      <c r="H192" s="12"/>
       <c r="I192" s="3"/>
       <c r="J192" s="3"/>
       <c r="K192" s="3"/>
@@ -4123,12 +4171,12 @@
     <row r="193" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A193" s="3"/>
       <c r="B193" s="3"/>
-      <c r="C193" s="3"/>
+      <c r="C193" s="16"/>
       <c r="D193" s="3"/>
       <c r="E193" s="6"/>
       <c r="F193" s="3"/>
       <c r="G193" s="3"/>
-      <c r="H193" s="3"/>
+      <c r="H193" s="12"/>
       <c r="I193" s="3"/>
       <c r="J193" s="3"/>
       <c r="K193" s="3"/>
@@ -4140,12 +4188,12 @@
     <row r="194" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A194" s="3"/>
       <c r="B194" s="3"/>
-      <c r="C194" s="3"/>
+      <c r="C194" s="16"/>
       <c r="D194" s="3"/>
       <c r="E194" s="6"/>
       <c r="F194" s="3"/>
       <c r="G194" s="3"/>
-      <c r="H194" s="3"/>
+      <c r="H194" s="12"/>
       <c r="I194" s="3"/>
       <c r="J194" s="3"/>
       <c r="K194" s="3"/>
@@ -4157,12 +4205,12 @@
     <row r="195" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A195" s="3"/>
       <c r="B195" s="3"/>
-      <c r="C195" s="3"/>
+      <c r="C195" s="16"/>
       <c r="D195" s="3"/>
       <c r="E195" s="6"/>
       <c r="F195" s="3"/>
       <c r="G195" s="3"/>
-      <c r="H195" s="3"/>
+      <c r="H195" s="12"/>
       <c r="I195" s="3"/>
       <c r="J195" s="3"/>
       <c r="K195" s="3"/>
@@ -4174,12 +4222,12 @@
     <row r="196" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A196" s="3"/>
       <c r="B196" s="3"/>
-      <c r="C196" s="3"/>
+      <c r="C196" s="16"/>
       <c r="D196" s="3"/>
       <c r="E196" s="6"/>
       <c r="F196" s="3"/>
       <c r="G196" s="3"/>
-      <c r="H196" s="3"/>
+      <c r="H196" s="12"/>
       <c r="I196" s="3"/>
       <c r="J196" s="3"/>
       <c r="K196" s="3"/>
@@ -4191,12 +4239,12 @@
     <row r="197" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A197" s="3"/>
       <c r="B197" s="3"/>
-      <c r="C197" s="3"/>
+      <c r="C197" s="16"/>
       <c r="D197" s="3"/>
       <c r="E197" s="6"/>
       <c r="F197" s="3"/>
       <c r="G197" s="3"/>
-      <c r="H197" s="3"/>
+      <c r="H197" s="12"/>
       <c r="I197" s="3"/>
       <c r="J197" s="3"/>
       <c r="K197" s="3"/>
@@ -4208,12 +4256,12 @@
     <row r="198" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A198" s="3"/>
       <c r="B198" s="3"/>
-      <c r="C198" s="3"/>
+      <c r="C198" s="16"/>
       <c r="D198" s="3"/>
       <c r="E198" s="6"/>
       <c r="F198" s="3"/>
       <c r="G198" s="3"/>
-      <c r="H198" s="3"/>
+      <c r="H198" s="12"/>
       <c r="I198" s="3"/>
       <c r="J198" s="3"/>
       <c r="K198" s="3"/>
@@ -4225,12 +4273,12 @@
     <row r="199" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A199" s="3"/>
       <c r="B199" s="3"/>
-      <c r="C199" s="3"/>
+      <c r="C199" s="16"/>
       <c r="D199" s="3"/>
       <c r="E199" s="6"/>
       <c r="F199" s="3"/>
       <c r="G199" s="3"/>
-      <c r="H199" s="3"/>
+      <c r="H199" s="12"/>
       <c r="I199" s="3"/>
       <c r="J199" s="3"/>
       <c r="K199" s="3"/>
@@ -4242,12 +4290,12 @@
     <row r="200" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A200" s="3"/>
       <c r="B200" s="3"/>
-      <c r="C200" s="3"/>
+      <c r="C200" s="16"/>
       <c r="D200" s="3"/>
       <c r="E200" s="6"/>
       <c r="F200" s="3"/>
       <c r="G200" s="3"/>
-      <c r="H200" s="3"/>
+      <c r="H200" s="12"/>
       <c r="I200" s="3"/>
       <c r="J200" s="3"/>
       <c r="K200" s="3"/>
@@ -4259,12 +4307,12 @@
     <row r="201" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A201" s="3"/>
       <c r="B201" s="3"/>
-      <c r="C201" s="3"/>
+      <c r="C201" s="16"/>
       <c r="D201" s="3"/>
       <c r="E201" s="6"/>
       <c r="F201" s="3"/>
       <c r="G201" s="3"/>
-      <c r="H201" s="3"/>
+      <c r="H201" s="12"/>
       <c r="I201" s="3"/>
       <c r="J201" s="3"/>
       <c r="K201" s="3"/>
@@ -4276,12 +4324,12 @@
     <row r="202" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A202" s="3"/>
       <c r="B202" s="3"/>
-      <c r="C202" s="3"/>
+      <c r="C202" s="16"/>
       <c r="D202" s="3"/>
       <c r="E202" s="6"/>
       <c r="F202" s="3"/>
       <c r="G202" s="3"/>
-      <c r="H202" s="3"/>
+      <c r="H202" s="12"/>
       <c r="I202" s="3"/>
       <c r="J202" s="3"/>
       <c r="K202" s="3"/>
@@ -4293,12 +4341,12 @@
     <row r="203" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A203" s="3"/>
       <c r="B203" s="3"/>
-      <c r="C203" s="3"/>
+      <c r="C203" s="16"/>
       <c r="D203" s="3"/>
       <c r="E203" s="6"/>
       <c r="F203" s="3"/>
       <c r="G203" s="3"/>
-      <c r="H203" s="3"/>
+      <c r="H203" s="12"/>
       <c r="I203" s="3"/>
       <c r="J203" s="3"/>
       <c r="K203" s="3"/>
@@ -4310,12 +4358,12 @@
     <row r="204" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A204" s="3"/>
       <c r="B204" s="3"/>
-      <c r="C204" s="3"/>
+      <c r="C204" s="16"/>
       <c r="D204" s="3"/>
       <c r="E204" s="6"/>
       <c r="F204" s="3"/>
       <c r="G204" s="3"/>
-      <c r="H204" s="3"/>
+      <c r="H204" s="12"/>
       <c r="I204" s="3"/>
       <c r="J204" s="3"/>
       <c r="K204" s="3"/>
@@ -4327,12 +4375,12 @@
     <row r="205" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A205" s="3"/>
       <c r="B205" s="3"/>
-      <c r="C205" s="3"/>
+      <c r="C205" s="16"/>
       <c r="D205" s="3"/>
       <c r="E205" s="6"/>
       <c r="F205" s="3"/>
       <c r="G205" s="3"/>
-      <c r="H205" s="3"/>
+      <c r="H205" s="12"/>
       <c r="I205" s="3"/>
       <c r="J205" s="3"/>
       <c r="K205" s="3"/>
@@ -4344,12 +4392,12 @@
     <row r="206" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A206" s="3"/>
       <c r="B206" s="3"/>
-      <c r="C206" s="3"/>
+      <c r="C206" s="16"/>
       <c r="D206" s="3"/>
       <c r="E206" s="6"/>
       <c r="F206" s="3"/>
       <c r="G206" s="3"/>
-      <c r="H206" s="3"/>
+      <c r="H206" s="12"/>
       <c r="I206" s="3"/>
       <c r="J206" s="3"/>
       <c r="K206" s="3"/>
@@ -4361,12 +4409,12 @@
     <row r="207" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A207" s="3"/>
       <c r="B207" s="3"/>
-      <c r="C207" s="3"/>
+      <c r="C207" s="16"/>
       <c r="D207" s="3"/>
       <c r="E207" s="6"/>
       <c r="F207" s="3"/>
       <c r="G207" s="3"/>
-      <c r="H207" s="3"/>
+      <c r="H207" s="12"/>
       <c r="I207" s="3"/>
       <c r="J207" s="3"/>
       <c r="K207" s="3"/>
@@ -4378,12 +4426,12 @@
     <row r="208" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A208" s="3"/>
       <c r="B208" s="3"/>
-      <c r="C208" s="3"/>
+      <c r="C208" s="16"/>
       <c r="D208" s="3"/>
       <c r="E208" s="6"/>
       <c r="F208" s="3"/>
       <c r="G208" s="3"/>
-      <c r="H208" s="3"/>
+      <c r="H208" s="12"/>
       <c r="I208" s="3"/>
       <c r="J208" s="3"/>
       <c r="K208" s="3"/>
@@ -4395,12 +4443,12 @@
     <row r="209" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A209" s="3"/>
       <c r="B209" s="3"/>
-      <c r="C209" s="3"/>
+      <c r="C209" s="16"/>
       <c r="D209" s="3"/>
       <c r="E209" s="6"/>
       <c r="F209" s="3"/>
       <c r="G209" s="3"/>
-      <c r="H209" s="3"/>
+      <c r="H209" s="12"/>
       <c r="I209" s="3"/>
       <c r="J209" s="3"/>
       <c r="K209" s="3"/>
@@ -4412,12 +4460,12 @@
     <row r="210" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A210" s="3"/>
       <c r="B210" s="3"/>
-      <c r="C210" s="3"/>
+      <c r="C210" s="16"/>
       <c r="D210" s="3"/>
       <c r="E210" s="6"/>
       <c r="F210" s="3"/>
       <c r="G210" s="3"/>
-      <c r="H210" s="3"/>
+      <c r="H210" s="12"/>
       <c r="I210" s="3"/>
       <c r="J210" s="3"/>
       <c r="K210" s="3"/>
@@ -4429,12 +4477,12 @@
     <row r="211" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A211" s="3"/>
       <c r="B211" s="3"/>
-      <c r="C211" s="3"/>
+      <c r="C211" s="16"/>
       <c r="D211" s="3"/>
       <c r="E211" s="6"/>
       <c r="F211" s="3"/>
       <c r="G211" s="3"/>
-      <c r="H211" s="3"/>
+      <c r="H211" s="12"/>
       <c r="I211" s="3"/>
       <c r="J211" s="3"/>
       <c r="K211" s="3"/>
@@ -4446,12 +4494,12 @@
     <row r="212" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A212" s="3"/>
       <c r="B212" s="3"/>
-      <c r="C212" s="3"/>
+      <c r="C212" s="16"/>
       <c r="D212" s="3"/>
       <c r="E212" s="6"/>
       <c r="F212" s="3"/>
       <c r="G212" s="3"/>
-      <c r="H212" s="3"/>
+      <c r="H212" s="12"/>
       <c r="I212" s="3"/>
       <c r="J212" s="3"/>
       <c r="K212" s="3"/>
@@ -4463,12 +4511,12 @@
     <row r="213" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A213" s="3"/>
       <c r="B213" s="3"/>
-      <c r="C213" s="3"/>
+      <c r="C213" s="16"/>
       <c r="D213" s="3"/>
       <c r="E213" s="6"/>
       <c r="F213" s="3"/>
       <c r="G213" s="3"/>
-      <c r="H213" s="3"/>
+      <c r="H213" s="12"/>
       <c r="I213" s="3"/>
       <c r="J213" s="3"/>
       <c r="K213" s="3"/>
@@ -4480,12 +4528,12 @@
     <row r="214" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A214" s="3"/>
       <c r="B214" s="3"/>
-      <c r="C214" s="3"/>
+      <c r="C214" s="16"/>
       <c r="D214" s="3"/>
       <c r="E214" s="6"/>
       <c r="F214" s="3"/>
       <c r="G214" s="3"/>
-      <c r="H214" s="3"/>
+      <c r="H214" s="12"/>
       <c r="I214" s="3"/>
       <c r="J214" s="3"/>
       <c r="K214" s="3"/>
@@ -4497,12 +4545,12 @@
     <row r="215" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A215" s="3"/>
       <c r="B215" s="3"/>
-      <c r="C215" s="3"/>
+      <c r="C215" s="16"/>
       <c r="D215" s="3"/>
       <c r="E215" s="6"/>
       <c r="F215" s="3"/>
       <c r="G215" s="3"/>
-      <c r="H215" s="3"/>
+      <c r="H215" s="12"/>
       <c r="I215" s="3"/>
       <c r="J215" s="3"/>
       <c r="K215" s="3"/>
@@ -4514,12 +4562,12 @@
     <row r="216" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A216" s="3"/>
       <c r="B216" s="3"/>
-      <c r="C216" s="3"/>
+      <c r="C216" s="16"/>
       <c r="D216" s="3"/>
       <c r="E216" s="6"/>
       <c r="F216" s="3"/>
       <c r="G216" s="3"/>
-      <c r="H216" s="3"/>
+      <c r="H216" s="12"/>
       <c r="I216" s="3"/>
       <c r="J216" s="3"/>
       <c r="K216" s="3"/>
@@ -4531,12 +4579,12 @@
     <row r="217" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A217" s="3"/>
       <c r="B217" s="3"/>
-      <c r="C217" s="3"/>
+      <c r="C217" s="16"/>
       <c r="D217" s="3"/>
       <c r="E217" s="6"/>
       <c r="F217" s="3"/>
       <c r="G217" s="3"/>
-      <c r="H217" s="3"/>
+      <c r="H217" s="12"/>
       <c r="I217" s="3"/>
       <c r="J217" s="3"/>
       <c r="K217" s="3"/>
@@ -4548,12 +4596,12 @@
     <row r="218" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A218" s="3"/>
       <c r="B218" s="3"/>
-      <c r="C218" s="3"/>
+      <c r="C218" s="16"/>
       <c r="D218" s="3"/>
       <c r="E218" s="6"/>
       <c r="F218" s="3"/>
       <c r="G218" s="3"/>
-      <c r="H218" s="3"/>
+      <c r="H218" s="12"/>
       <c r="I218" s="3"/>
       <c r="J218" s="3"/>
       <c r="K218" s="3"/>
@@ -4565,12 +4613,12 @@
     <row r="219" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A219" s="3"/>
       <c r="B219" s="3"/>
-      <c r="C219" s="3"/>
+      <c r="C219" s="16"/>
       <c r="D219" s="3"/>
       <c r="E219" s="6"/>
       <c r="F219" s="3"/>
       <c r="G219" s="3"/>
-      <c r="H219" s="3"/>
+      <c r="H219" s="12"/>
       <c r="I219" s="3"/>
       <c r="J219" s="3"/>
       <c r="K219" s="3"/>
@@ -4582,12 +4630,12 @@
     <row r="220" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A220" s="3"/>
       <c r="B220" s="3"/>
-      <c r="C220" s="3"/>
+      <c r="C220" s="16"/>
       <c r="D220" s="3"/>
       <c r="E220" s="6"/>
       <c r="F220" s="3"/>
       <c r="G220" s="3"/>
-      <c r="H220" s="3"/>
+      <c r="H220" s="12"/>
       <c r="I220" s="3"/>
       <c r="J220" s="3"/>
       <c r="K220" s="3"/>
@@ -4599,12 +4647,12 @@
     <row r="221" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A221" s="3"/>
       <c r="B221" s="3"/>
-      <c r="C221" s="3"/>
+      <c r="C221" s="16"/>
       <c r="D221" s="3"/>
       <c r="E221" s="6"/>
       <c r="F221" s="3"/>
       <c r="G221" s="3"/>
-      <c r="H221" s="3"/>
+      <c r="H221" s="12"/>
       <c r="I221" s="3"/>
       <c r="J221" s="3"/>
       <c r="K221" s="3"/>
@@ -4616,12 +4664,12 @@
     <row r="222" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A222" s="3"/>
       <c r="B222" s="3"/>
-      <c r="C222" s="3"/>
+      <c r="C222" s="16"/>
       <c r="D222" s="3"/>
       <c r="E222" s="6"/>
       <c r="F222" s="3"/>
       <c r="G222" s="3"/>
-      <c r="H222" s="3"/>
+      <c r="H222" s="12"/>
       <c r="I222" s="3"/>
       <c r="J222" s="3"/>
       <c r="K222" s="3"/>
@@ -4633,12 +4681,12 @@
     <row r="223" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A223" s="3"/>
       <c r="B223" s="3"/>
-      <c r="C223" s="3"/>
+      <c r="C223" s="16"/>
       <c r="D223" s="3"/>
       <c r="E223" s="6"/>
       <c r="F223" s="3"/>
       <c r="G223" s="3"/>
-      <c r="H223" s="3"/>
+      <c r="H223" s="12"/>
       <c r="I223" s="3"/>
       <c r="J223" s="3"/>
       <c r="K223" s="3"/>
@@ -4650,12 +4698,12 @@
     <row r="224" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A224" s="3"/>
       <c r="B224" s="3"/>
-      <c r="C224" s="3"/>
+      <c r="C224" s="16"/>
       <c r="D224" s="3"/>
       <c r="E224" s="6"/>
       <c r="F224" s="3"/>
       <c r="G224" s="3"/>
-      <c r="H224" s="3"/>
+      <c r="H224" s="12"/>
       <c r="I224" s="3"/>
       <c r="J224" s="3"/>
       <c r="K224" s="3"/>
@@ -4667,12 +4715,12 @@
     <row r="225" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A225" s="3"/>
       <c r="B225" s="3"/>
-      <c r="C225" s="3"/>
+      <c r="C225" s="16"/>
       <c r="D225" s="3"/>
       <c r="E225" s="6"/>
       <c r="F225" s="3"/>
       <c r="G225" s="3"/>
-      <c r="H225" s="3"/>
+      <c r="H225" s="12"/>
       <c r="I225" s="3"/>
       <c r="J225" s="3"/>
       <c r="K225" s="3"/>
@@ -4684,12 +4732,12 @@
     <row r="226" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A226" s="3"/>
       <c r="B226" s="3"/>
-      <c r="C226" s="3"/>
+      <c r="C226" s="16"/>
       <c r="D226" s="3"/>
       <c r="E226" s="6"/>
       <c r="F226" s="3"/>
       <c r="G226" s="3"/>
-      <c r="H226" s="3"/>
+      <c r="H226" s="12"/>
       <c r="I226" s="3"/>
       <c r="J226" s="3"/>
       <c r="K226" s="3"/>
@@ -4701,12 +4749,12 @@
     <row r="227" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A227" s="3"/>
       <c r="B227" s="3"/>
-      <c r="C227" s="3"/>
+      <c r="C227" s="16"/>
       <c r="D227" s="3"/>
       <c r="E227" s="6"/>
       <c r="F227" s="3"/>
       <c r="G227" s="3"/>
-      <c r="H227" s="3"/>
+      <c r="H227" s="12"/>
       <c r="I227" s="3"/>
       <c r="J227" s="3"/>
       <c r="K227" s="3"/>
@@ -4718,12 +4766,12 @@
     <row r="228" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A228" s="3"/>
       <c r="B228" s="3"/>
-      <c r="C228" s="3"/>
+      <c r="C228" s="16"/>
       <c r="D228" s="3"/>
       <c r="E228" s="6"/>
       <c r="F228" s="3"/>
       <c r="G228" s="3"/>
-      <c r="H228" s="3"/>
+      <c r="H228" s="12"/>
       <c r="I228" s="3"/>
       <c r="J228" s="3"/>
       <c r="K228" s="3"/>
@@ -4735,12 +4783,12 @@
     <row r="229" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A229" s="3"/>
       <c r="B229" s="3"/>
-      <c r="C229" s="3"/>
+      <c r="C229" s="16"/>
       <c r="D229" s="3"/>
       <c r="E229" s="6"/>
       <c r="F229" s="3"/>
       <c r="G229" s="3"/>
-      <c r="H229" s="3"/>
+      <c r="H229" s="12"/>
       <c r="I229" s="3"/>
       <c r="J229" s="3"/>
       <c r="K229" s="3"/>
@@ -4752,12 +4800,12 @@
     <row r="230" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A230" s="3"/>
       <c r="B230" s="3"/>
-      <c r="C230" s="3"/>
+      <c r="C230" s="16"/>
       <c r="D230" s="3"/>
       <c r="E230" s="6"/>
       <c r="F230" s="3"/>
       <c r="G230" s="3"/>
-      <c r="H230" s="3"/>
+      <c r="H230" s="12"/>
       <c r="I230" s="3"/>
       <c r="J230" s="3"/>
       <c r="K230" s="3"/>
@@ -4769,12 +4817,12 @@
     <row r="231" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A231" s="3"/>
       <c r="B231" s="3"/>
-      <c r="C231" s="3"/>
+      <c r="C231" s="16"/>
       <c r="D231" s="3"/>
       <c r="E231" s="6"/>
       <c r="F231" s="3"/>
       <c r="G231" s="3"/>
-      <c r="H231" s="3"/>
+      <c r="H231" s="12"/>
       <c r="I231" s="3"/>
       <c r="J231" s="3"/>
       <c r="K231" s="3"/>
@@ -4786,12 +4834,12 @@
     <row r="232" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A232" s="3"/>
       <c r="B232" s="3"/>
-      <c r="C232" s="3"/>
+      <c r="C232" s="16"/>
       <c r="D232" s="3"/>
       <c r="E232" s="6"/>
       <c r="F232" s="3"/>
       <c r="G232" s="3"/>
-      <c r="H232" s="3"/>
+      <c r="H232" s="12"/>
       <c r="I232" s="3"/>
       <c r="J232" s="3"/>
       <c r="K232" s="3"/>
@@ -4803,12 +4851,12 @@
     <row r="233" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A233" s="3"/>
       <c r="B233" s="3"/>
-      <c r="C233" s="3"/>
+      <c r="C233" s="16"/>
       <c r="D233" s="3"/>
       <c r="E233" s="6"/>
       <c r="F233" s="3"/>
       <c r="G233" s="3"/>
-      <c r="H233" s="3"/>
+      <c r="H233" s="12"/>
       <c r="I233" s="3"/>
       <c r="J233" s="3"/>
       <c r="K233" s="3"/>
@@ -4820,12 +4868,12 @@
     <row r="234" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A234" s="3"/>
       <c r="B234" s="3"/>
-      <c r="C234" s="3"/>
+      <c r="C234" s="16"/>
       <c r="D234" s="3"/>
       <c r="E234" s="6"/>
       <c r="F234" s="3"/>
       <c r="G234" s="3"/>
-      <c r="H234" s="3"/>
+      <c r="H234" s="12"/>
       <c r="I234" s="3"/>
       <c r="J234" s="3"/>
       <c r="K234" s="3"/>
@@ -4837,12 +4885,12 @@
     <row r="235" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A235" s="3"/>
       <c r="B235" s="3"/>
-      <c r="C235" s="3"/>
+      <c r="C235" s="16"/>
       <c r="D235" s="3"/>
       <c r="E235" s="6"/>
       <c r="F235" s="3"/>
       <c r="G235" s="3"/>
-      <c r="H235" s="3"/>
+      <c r="H235" s="12"/>
       <c r="I235" s="3"/>
       <c r="J235" s="3"/>
       <c r="K235" s="3"/>
@@ -4854,12 +4902,12 @@
     <row r="236" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A236" s="3"/>
       <c r="B236" s="3"/>
-      <c r="C236" s="3"/>
+      <c r="C236" s="16"/>
       <c r="D236" s="3"/>
       <c r="E236" s="6"/>
       <c r="F236" s="3"/>
       <c r="G236" s="3"/>
-      <c r="H236" s="3"/>
+      <c r="H236" s="12"/>
       <c r="I236" s="3"/>
       <c r="J236" s="3"/>
       <c r="K236" s="3"/>
@@ -4871,12 +4919,12 @@
     <row r="237" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A237" s="3"/>
       <c r="B237" s="3"/>
-      <c r="C237" s="3"/>
+      <c r="C237" s="16"/>
       <c r="D237" s="3"/>
       <c r="E237" s="6"/>
       <c r="F237" s="3"/>
       <c r="G237" s="3"/>
-      <c r="H237" s="3"/>
+      <c r="H237" s="12"/>
       <c r="I237" s="3"/>
       <c r="J237" s="3"/>
       <c r="K237" s="3"/>
@@ -4888,12 +4936,12 @@
     <row r="238" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A238" s="3"/>
       <c r="B238" s="3"/>
-      <c r="C238" s="3"/>
+      <c r="C238" s="16"/>
       <c r="D238" s="3"/>
       <c r="E238" s="6"/>
       <c r="F238" s="3"/>
       <c r="G238" s="3"/>
-      <c r="H238" s="3"/>
+      <c r="H238" s="12"/>
       <c r="I238" s="3"/>
       <c r="J238" s="3"/>
       <c r="K238" s="3"/>
@@ -4905,12 +4953,12 @@
     <row r="239" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A239" s="3"/>
       <c r="B239" s="3"/>
-      <c r="C239" s="3"/>
+      <c r="C239" s="16"/>
       <c r="D239" s="3"/>
       <c r="E239" s="6"/>
       <c r="F239" s="3"/>
       <c r="G239" s="3"/>
-      <c r="H239" s="3"/>
+      <c r="H239" s="12"/>
       <c r="I239" s="3"/>
       <c r="J239" s="3"/>
       <c r="K239" s="3"/>
@@ -4922,12 +4970,12 @@
     <row r="240" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A240" s="3"/>
       <c r="B240" s="3"/>
-      <c r="C240" s="3"/>
+      <c r="C240" s="16"/>
       <c r="D240" s="3"/>
       <c r="E240" s="6"/>
       <c r="F240" s="3"/>
       <c r="G240" s="3"/>
-      <c r="H240" s="3"/>
+      <c r="H240" s="12"/>
       <c r="I240" s="3"/>
       <c r="J240" s="3"/>
       <c r="K240" s="3"/>
@@ -4939,12 +4987,12 @@
     <row r="241" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A241" s="3"/>
       <c r="B241" s="3"/>
-      <c r="C241" s="3"/>
+      <c r="C241" s="16"/>
       <c r="D241" s="3"/>
       <c r="E241" s="6"/>
       <c r="F241" s="3"/>
       <c r="G241" s="3"/>
-      <c r="H241" s="3"/>
+      <c r="H241" s="12"/>
       <c r="I241" s="3"/>
       <c r="J241" s="3"/>
       <c r="K241" s="3"/>
@@ -4956,12 +5004,12 @@
     <row r="242" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A242" s="3"/>
       <c r="B242" s="3"/>
-      <c r="C242" s="3"/>
+      <c r="C242" s="16"/>
       <c r="D242" s="3"/>
       <c r="E242" s="6"/>
       <c r="F242" s="3"/>
       <c r="G242" s="3"/>
-      <c r="H242" s="3"/>
+      <c r="H242" s="12"/>
       <c r="I242" s="3"/>
       <c r="J242" s="3"/>
       <c r="K242" s="3"/>
@@ -4973,12 +5021,12 @@
     <row r="243" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A243" s="3"/>
       <c r="B243" s="3"/>
-      <c r="C243" s="3"/>
+      <c r="C243" s="16"/>
       <c r="D243" s="3"/>
       <c r="E243" s="6"/>
       <c r="F243" s="3"/>
       <c r="G243" s="3"/>
-      <c r="H243" s="3"/>
+      <c r="H243" s="12"/>
       <c r="I243" s="3"/>
       <c r="J243" s="3"/>
       <c r="K243" s="3"/>
@@ -4990,12 +5038,12 @@
     <row r="244" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A244" s="3"/>
       <c r="B244" s="3"/>
-      <c r="C244" s="3"/>
+      <c r="C244" s="16"/>
       <c r="D244" s="3"/>
       <c r="E244" s="6"/>
       <c r="F244" s="3"/>
       <c r="G244" s="3"/>
-      <c r="H244" s="3"/>
+      <c r="H244" s="12"/>
       <c r="I244" s="3"/>
       <c r="J244" s="3"/>
       <c r="K244" s="3"/>
@@ -5007,12 +5055,12 @@
     <row r="245" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A245" s="3"/>
       <c r="B245" s="3"/>
-      <c r="C245" s="3"/>
+      <c r="C245" s="16"/>
       <c r="D245" s="3"/>
       <c r="E245" s="6"/>
       <c r="F245" s="3"/>
       <c r="G245" s="3"/>
-      <c r="H245" s="3"/>
+      <c r="H245" s="12"/>
       <c r="I245" s="3"/>
       <c r="J245" s="3"/>
       <c r="K245" s="3"/>
@@ -5024,12 +5072,12 @@
     <row r="246" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A246" s="3"/>
       <c r="B246" s="3"/>
-      <c r="C246" s="3"/>
+      <c r="C246" s="16"/>
       <c r="D246" s="3"/>
       <c r="E246" s="6"/>
       <c r="F246" s="3"/>
       <c r="G246" s="3"/>
-      <c r="H246" s="3"/>
+      <c r="H246" s="12"/>
       <c r="I246" s="3"/>
       <c r="J246" s="3"/>
       <c r="K246" s="3"/>
@@ -5041,12 +5089,12 @@
     <row r="247" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A247" s="3"/>
       <c r="B247" s="3"/>
-      <c r="C247" s="3"/>
+      <c r="C247" s="16"/>
       <c r="D247" s="3"/>
       <c r="E247" s="6"/>
       <c r="F247" s="3"/>
       <c r="G247" s="3"/>
-      <c r="H247" s="3"/>
+      <c r="H247" s="12"/>
       <c r="I247" s="3"/>
       <c r="J247" s="3"/>
       <c r="K247" s="3"/>
@@ -5058,12 +5106,12 @@
     <row r="248" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A248" s="3"/>
       <c r="B248" s="3"/>
-      <c r="C248" s="3"/>
+      <c r="C248" s="16"/>
       <c r="D248" s="3"/>
       <c r="E248" s="6"/>
       <c r="F248" s="3"/>
       <c r="G248" s="3"/>
-      <c r="H248" s="3"/>
+      <c r="H248" s="12"/>
       <c r="I248" s="3"/>
       <c r="J248" s="3"/>
       <c r="K248" s="3"/>
@@ -5075,12 +5123,12 @@
     <row r="249" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A249" s="3"/>
       <c r="B249" s="3"/>
-      <c r="C249" s="3"/>
+      <c r="C249" s="16"/>
       <c r="D249" s="3"/>
       <c r="E249" s="6"/>
       <c r="F249" s="3"/>
       <c r="G249" s="3"/>
-      <c r="H249" s="3"/>
+      <c r="H249" s="12"/>
       <c r="I249" s="3"/>
       <c r="J249" s="3"/>
       <c r="K249" s="3"/>
@@ -5092,12 +5140,12 @@
     <row r="250" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A250" s="3"/>
       <c r="B250" s="3"/>
-      <c r="C250" s="3"/>
+      <c r="C250" s="16"/>
       <c r="D250" s="3"/>
       <c r="E250" s="6"/>
       <c r="F250" s="3"/>
       <c r="G250" s="3"/>
-      <c r="H250" s="3"/>
+      <c r="H250" s="12"/>
       <c r="I250" s="3"/>
       <c r="J250" s="3"/>
       <c r="K250" s="3"/>
@@ -5109,12 +5157,12 @@
     <row r="251" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A251" s="3"/>
       <c r="B251" s="3"/>
-      <c r="C251" s="3"/>
+      <c r="C251" s="16"/>
       <c r="D251" s="3"/>
       <c r="E251" s="6"/>
       <c r="F251" s="3"/>
       <c r="G251" s="3"/>
-      <c r="H251" s="3"/>
+      <c r="H251" s="12"/>
       <c r="I251" s="3"/>
       <c r="J251" s="3"/>
       <c r="K251" s="3"/>
@@ -5126,12 +5174,12 @@
     <row r="252" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A252" s="3"/>
       <c r="B252" s="3"/>
-      <c r="C252" s="3"/>
+      <c r="C252" s="16"/>
       <c r="D252" s="3"/>
       <c r="E252" s="6"/>
       <c r="F252" s="3"/>
       <c r="G252" s="3"/>
-      <c r="H252" s="3"/>
+      <c r="H252" s="12"/>
       <c r="I252" s="3"/>
       <c r="J252" s="3"/>
       <c r="K252" s="3"/>
@@ -5143,12 +5191,12 @@
     <row r="253" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A253" s="3"/>
       <c r="B253" s="3"/>
-      <c r="C253" s="3"/>
+      <c r="C253" s="16"/>
       <c r="D253" s="3"/>
       <c r="E253" s="6"/>
       <c r="F253" s="3"/>
       <c r="G253" s="3"/>
-      <c r="H253" s="3"/>
+      <c r="H253" s="12"/>
       <c r="I253" s="3"/>
       <c r="J253" s="3"/>
       <c r="K253" s="3"/>
@@ -5160,12 +5208,12 @@
     <row r="254" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A254" s="3"/>
       <c r="B254" s="3"/>
-      <c r="C254" s="3"/>
+      <c r="C254" s="16"/>
       <c r="D254" s="3"/>
       <c r="E254" s="6"/>
       <c r="F254" s="3"/>
       <c r="G254" s="3"/>
-      <c r="H254" s="3"/>
+      <c r="H254" s="12"/>
       <c r="I254" s="3"/>
       <c r="J254" s="3"/>
       <c r="K254" s="3"/>
@@ -5177,12 +5225,12 @@
     <row r="255" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A255" s="3"/>
       <c r="B255" s="3"/>
-      <c r="C255" s="3"/>
+      <c r="C255" s="16"/>
       <c r="D255" s="3"/>
       <c r="E255" s="6"/>
       <c r="F255" s="3"/>
       <c r="G255" s="3"/>
-      <c r="H255" s="3"/>
+      <c r="H255" s="12"/>
       <c r="I255" s="3"/>
       <c r="J255" s="3"/>
       <c r="K255" s="3"/>
@@ -5194,12 +5242,12 @@
     <row r="256" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A256" s="3"/>
       <c r="B256" s="3"/>
-      <c r="C256" s="3"/>
+      <c r="C256" s="16"/>
       <c r="D256" s="3"/>
       <c r="E256" s="6"/>
       <c r="F256" s="3"/>
       <c r="G256" s="3"/>
-      <c r="H256" s="3"/>
+      <c r="H256" s="12"/>
       <c r="I256" s="3"/>
       <c r="J256" s="3"/>
       <c r="K256" s="3"/>
@@ -5211,12 +5259,12 @@
     <row r="257" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A257" s="3"/>
       <c r="B257" s="3"/>
-      <c r="C257" s="3"/>
+      <c r="C257" s="16"/>
       <c r="D257" s="3"/>
       <c r="E257" s="6"/>
       <c r="F257" s="3"/>
       <c r="G257" s="3"/>
-      <c r="H257" s="3"/>
+      <c r="H257" s="12"/>
       <c r="I257" s="3"/>
       <c r="J257" s="3"/>
       <c r="K257" s="3"/>
@@ -5228,12 +5276,12 @@
     <row r="258" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A258" s="3"/>
       <c r="B258" s="3"/>
-      <c r="C258" s="3"/>
+      <c r="C258" s="16"/>
       <c r="D258" s="3"/>
       <c r="E258" s="6"/>
       <c r="F258" s="3"/>
       <c r="G258" s="3"/>
-      <c r="H258" s="3"/>
+      <c r="H258" s="12"/>
       <c r="I258" s="3"/>
       <c r="J258" s="3"/>
       <c r="K258" s="3"/>
@@ -5245,12 +5293,12 @@
     <row r="259" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A259" s="3"/>
       <c r="B259" s="3"/>
-      <c r="C259" s="3"/>
+      <c r="C259" s="16"/>
       <c r="D259" s="3"/>
       <c r="E259" s="6"/>
       <c r="F259" s="3"/>
       <c r="G259" s="3"/>
-      <c r="H259" s="3"/>
+      <c r="H259" s="12"/>
       <c r="I259" s="3"/>
       <c r="J259" s="3"/>
       <c r="K259" s="3"/>
@@ -5262,12 +5310,12 @@
     <row r="260" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A260" s="3"/>
       <c r="B260" s="3"/>
-      <c r="C260" s="3"/>
+      <c r="C260" s="16"/>
       <c r="D260" s="3"/>
       <c r="E260" s="6"/>
       <c r="F260" s="3"/>
       <c r="G260" s="3"/>
-      <c r="H260" s="3"/>
+      <c r="H260" s="12"/>
       <c r="I260" s="3"/>
       <c r="J260" s="3"/>
       <c r="K260" s="3"/>
@@ -5279,12 +5327,12 @@
     <row r="261" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A261" s="3"/>
       <c r="B261" s="3"/>
-      <c r="C261" s="3"/>
+      <c r="C261" s="16"/>
       <c r="D261" s="3"/>
       <c r="E261" s="6"/>
       <c r="F261" s="3"/>
       <c r="G261" s="3"/>
-      <c r="H261" s="3"/>
+      <c r="H261" s="12"/>
       <c r="I261" s="3"/>
       <c r="J261" s="3"/>
       <c r="K261" s="3"/>
@@ -5296,12 +5344,12 @@
     <row r="262" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A262" s="3"/>
       <c r="B262" s="3"/>
-      <c r="C262" s="3"/>
+      <c r="C262" s="16"/>
       <c r="D262" s="3"/>
       <c r="E262" s="6"/>
       <c r="F262" s="3"/>
       <c r="G262" s="3"/>
-      <c r="H262" s="3"/>
+      <c r="H262" s="12"/>
       <c r="I262" s="3"/>
       <c r="J262" s="3"/>
       <c r="K262" s="3"/>
@@ -5313,12 +5361,12 @@
     <row r="263" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A263" s="3"/>
       <c r="B263" s="3"/>
-      <c r="C263" s="3"/>
+      <c r="C263" s="16"/>
       <c r="D263" s="3"/>
       <c r="E263" s="6"/>
       <c r="F263" s="3"/>
       <c r="G263" s="3"/>
-      <c r="H263" s="3"/>
+      <c r="H263" s="12"/>
       <c r="I263" s="3"/>
       <c r="J263" s="3"/>
       <c r="K263" s="3"/>
@@ -5330,12 +5378,12 @@
     <row r="264" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A264" s="3"/>
       <c r="B264" s="3"/>
-      <c r="C264" s="3"/>
+      <c r="C264" s="16"/>
       <c r="D264" s="3"/>
       <c r="E264" s="6"/>
       <c r="F264" s="3"/>
       <c r="G264" s="3"/>
-      <c r="H264" s="3"/>
+      <c r="H264" s="12"/>
       <c r="I264" s="3"/>
       <c r="J264" s="3"/>
       <c r="K264" s="3"/>
@@ -5347,12 +5395,12 @@
     <row r="265" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A265" s="3"/>
       <c r="B265" s="3"/>
-      <c r="C265" s="3"/>
+      <c r="C265" s="16"/>
       <c r="D265" s="3"/>
       <c r="E265" s="6"/>
       <c r="F265" s="3"/>
       <c r="G265" s="3"/>
-      <c r="H265" s="3"/>
+      <c r="H265" s="12"/>
       <c r="I265" s="3"/>
       <c r="J265" s="3"/>
       <c r="K265" s="3"/>
@@ -5364,12 +5412,12 @@
     <row r="266" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A266" s="3"/>
       <c r="B266" s="3"/>
-      <c r="C266" s="3"/>
+      <c r="C266" s="16"/>
       <c r="D266" s="3"/>
       <c r="E266" s="6"/>
       <c r="F266" s="3"/>
       <c r="G266" s="3"/>
-      <c r="H266" s="3"/>
+      <c r="H266" s="12"/>
       <c r="I266" s="3"/>
       <c r="J266" s="3"/>
       <c r="K266" s="3"/>
@@ -5381,12 +5429,12 @@
     <row r="267" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A267" s="3"/>
       <c r="B267" s="3"/>
-      <c r="C267" s="3"/>
+      <c r="C267" s="16"/>
       <c r="D267" s="3"/>
       <c r="E267" s="6"/>
       <c r="F267" s="3"/>
       <c r="G267" s="3"/>
-      <c r="H267" s="3"/>
+      <c r="H267" s="12"/>
       <c r="I267" s="3"/>
       <c r="J267" s="3"/>
       <c r="K267" s="3"/>
@@ -5398,12 +5446,12 @@
     <row r="268" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A268" s="3"/>
       <c r="B268" s="3"/>
-      <c r="C268" s="3"/>
+      <c r="C268" s="16"/>
       <c r="D268" s="3"/>
       <c r="E268" s="6"/>
       <c r="F268" s="3"/>
       <c r="G268" s="3"/>
-      <c r="H268" s="3"/>
+      <c r="H268" s="12"/>
       <c r="I268" s="3"/>
       <c r="J268" s="3"/>
       <c r="K268" s="3"/>
@@ -5415,12 +5463,12 @@
     <row r="269" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A269" s="3"/>
       <c r="B269" s="3"/>
-      <c r="C269" s="3"/>
+      <c r="C269" s="16"/>
       <c r="D269" s="3"/>
       <c r="E269" s="6"/>
       <c r="F269" s="3"/>
       <c r="G269" s="3"/>
-      <c r="H269" s="3"/>
+      <c r="H269" s="12"/>
       <c r="I269" s="3"/>
       <c r="J269" s="3"/>
       <c r="K269" s="3"/>
@@ -5432,12 +5480,12 @@
     <row r="270" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A270" s="3"/>
       <c r="B270" s="3"/>
-      <c r="C270" s="3"/>
+      <c r="C270" s="16"/>
       <c r="D270" s="3"/>
       <c r="E270" s="6"/>
       <c r="F270" s="3"/>
       <c r="G270" s="3"/>
-      <c r="H270" s="3"/>
+      <c r="H270" s="12"/>
       <c r="I270" s="3"/>
       <c r="J270" s="3"/>
       <c r="K270" s="3"/>
@@ -5449,12 +5497,12 @@
     <row r="271" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A271" s="3"/>
       <c r="B271" s="3"/>
-      <c r="C271" s="3"/>
+      <c r="C271" s="16"/>
       <c r="D271" s="3"/>
       <c r="E271" s="6"/>
       <c r="F271" s="3"/>
       <c r="G271" s="3"/>
-      <c r="H271" s="3"/>
+      <c r="H271" s="12"/>
       <c r="I271" s="3"/>
       <c r="J271" s="3"/>
       <c r="K271" s="3"/>
@@ -5466,12 +5514,12 @@
     <row r="272" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A272" s="3"/>
       <c r="B272" s="3"/>
-      <c r="C272" s="3"/>
+      <c r="C272" s="16"/>
       <c r="D272" s="3"/>
       <c r="E272" s="6"/>
       <c r="F272" s="3"/>
       <c r="G272" s="3"/>
-      <c r="H272" s="3"/>
+      <c r="H272" s="12"/>
       <c r="I272" s="3"/>
       <c r="J272" s="3"/>
       <c r="K272" s="3"/>
@@ -5483,12 +5531,12 @@
     <row r="273" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A273" s="3"/>
       <c r="B273" s="3"/>
-      <c r="C273" s="3"/>
+      <c r="C273" s="16"/>
       <c r="D273" s="3"/>
       <c r="E273" s="6"/>
       <c r="F273" s="3"/>
       <c r="G273" s="3"/>
-      <c r="H273" s="3"/>
+      <c r="H273" s="12"/>
       <c r="I273" s="3"/>
       <c r="J273" s="3"/>
       <c r="K273" s="3"/>
@@ -5500,12 +5548,12 @@
     <row r="274" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A274" s="3"/>
       <c r="B274" s="3"/>
-      <c r="C274" s="3"/>
+      <c r="C274" s="16"/>
       <c r="D274" s="3"/>
       <c r="E274" s="6"/>
       <c r="F274" s="3"/>
       <c r="G274" s="3"/>
-      <c r="H274" s="3"/>
+      <c r="H274" s="12"/>
       <c r="I274" s="3"/>
       <c r="J274" s="3"/>
       <c r="K274" s="3"/>
@@ -5517,12 +5565,12 @@
     <row r="275" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A275" s="3"/>
       <c r="B275" s="3"/>
-      <c r="C275" s="3"/>
+      <c r="C275" s="16"/>
       <c r="D275" s="3"/>
       <c r="E275" s="6"/>
       <c r="F275" s="3"/>
       <c r="G275" s="3"/>
-      <c r="H275" s="3"/>
+      <c r="H275" s="12"/>
       <c r="I275" s="3"/>
       <c r="J275" s="3"/>
       <c r="K275" s="3"/>
@@ -5534,12 +5582,12 @@
     <row r="276" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A276" s="3"/>
       <c r="B276" s="3"/>
-      <c r="C276" s="3"/>
+      <c r="C276" s="16"/>
       <c r="D276" s="3"/>
       <c r="E276" s="6"/>
       <c r="F276" s="3"/>
       <c r="G276" s="3"/>
-      <c r="H276" s="3"/>
+      <c r="H276" s="12"/>
       <c r="I276" s="3"/>
       <c r="J276" s="3"/>
       <c r="K276" s="3"/>
@@ -5551,12 +5599,12 @@
     <row r="277" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A277" s="3"/>
       <c r="B277" s="3"/>
-      <c r="C277" s="3"/>
+      <c r="C277" s="16"/>
       <c r="D277" s="3"/>
       <c r="E277" s="6"/>
       <c r="F277" s="3"/>
       <c r="G277" s="3"/>
-      <c r="H277" s="3"/>
+      <c r="H277" s="12"/>
       <c r="I277" s="3"/>
       <c r="J277" s="3"/>
       <c r="K277" s="3"/>
@@ -5568,12 +5616,12 @@
     <row r="278" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A278" s="3"/>
       <c r="B278" s="3"/>
-      <c r="C278" s="3"/>
+      <c r="C278" s="16"/>
       <c r="D278" s="3"/>
       <c r="E278" s="6"/>
       <c r="F278" s="3"/>
       <c r="G278" s="3"/>
-      <c r="H278" s="3"/>
+      <c r="H278" s="12"/>
       <c r="I278" s="3"/>
       <c r="J278" s="3"/>
       <c r="K278" s="3"/>
@@ -5585,12 +5633,12 @@
     <row r="279" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A279" s="3"/>
       <c r="B279" s="3"/>
-      <c r="C279" s="3"/>
+      <c r="C279" s="16"/>
       <c r="D279" s="3"/>
       <c r="E279" s="6"/>
       <c r="F279" s="3"/>
       <c r="G279" s="3"/>
-      <c r="H279" s="3"/>
+      <c r="H279" s="12"/>
       <c r="I279" s="3"/>
       <c r="J279" s="3"/>
       <c r="K279" s="3"/>
@@ -5602,12 +5650,12 @@
     <row r="280" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A280" s="3"/>
       <c r="B280" s="3"/>
-      <c r="C280" s="3"/>
+      <c r="C280" s="16"/>
       <c r="D280" s="3"/>
       <c r="E280" s="6"/>
       <c r="F280" s="3"/>
       <c r="G280" s="3"/>
-      <c r="H280" s="3"/>
+      <c r="H280" s="12"/>
       <c r="I280" s="3"/>
       <c r="J280" s="3"/>
       <c r="K280" s="3"/>
@@ -5619,12 +5667,12 @@
     <row r="281" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A281" s="3"/>
       <c r="B281" s="3"/>
-      <c r="C281" s="3"/>
+      <c r="C281" s="16"/>
       <c r="D281" s="3"/>
       <c r="E281" s="6"/>
       <c r="F281" s="3"/>
       <c r="G281" s="3"/>
-      <c r="H281" s="3"/>
+      <c r="H281" s="12"/>
       <c r="I281" s="3"/>
       <c r="J281" s="3"/>
       <c r="K281" s="3"/>
@@ -5636,12 +5684,12 @@
     <row r="282" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A282" s="3"/>
       <c r="B282" s="3"/>
-      <c r="C282" s="3"/>
+      <c r="C282" s="16"/>
       <c r="D282" s="3"/>
       <c r="E282" s="6"/>
       <c r="F282" s="3"/>
       <c r="G282" s="3"/>
-      <c r="H282" s="3"/>
+      <c r="H282" s="12"/>
       <c r="I282" s="3"/>
       <c r="J282" s="3"/>
       <c r="K282" s="3"/>
@@ -5653,12 +5701,12 @@
     <row r="283" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A283" s="3"/>
       <c r="B283" s="3"/>
-      <c r="C283" s="3"/>
+      <c r="C283" s="16"/>
       <c r="D283" s="3"/>
       <c r="E283" s="6"/>
       <c r="F283" s="3"/>
       <c r="G283" s="3"/>
-      <c r="H283" s="3"/>
+      <c r="H283" s="12"/>
       <c r="I283" s="3"/>
       <c r="J283" s="3"/>
       <c r="K283" s="3"/>
@@ -5670,12 +5718,12 @@
     <row r="284" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A284" s="3"/>
       <c r="B284" s="3"/>
-      <c r="C284" s="3"/>
+      <c r="C284" s="16"/>
       <c r="D284" s="3"/>
       <c r="E284" s="6"/>
       <c r="F284" s="3"/>
       <c r="G284" s="3"/>
-      <c r="H284" s="3"/>
+      <c r="H284" s="12"/>
       <c r="I284" s="3"/>
       <c r="J284" s="3"/>
       <c r="K284" s="3"/>
@@ -5687,12 +5735,12 @@
     <row r="285" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A285" s="3"/>
       <c r="B285" s="3"/>
-      <c r="C285" s="3"/>
+      <c r="C285" s="16"/>
       <c r="D285" s="3"/>
       <c r="E285" s="6"/>
       <c r="F285" s="3"/>
       <c r="G285" s="3"/>
-      <c r="H285" s="3"/>
+      <c r="H285" s="12"/>
       <c r="I285" s="3"/>
       <c r="J285" s="3"/>
       <c r="K285" s="3"/>
@@ -5704,12 +5752,12 @@
     <row r="286" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A286" s="3"/>
       <c r="B286" s="3"/>
-      <c r="C286" s="3"/>
+      <c r="C286" s="16"/>
       <c r="D286" s="3"/>
       <c r="E286" s="6"/>
       <c r="F286" s="3"/>
       <c r="G286" s="3"/>
-      <c r="H286" s="3"/>
+      <c r="H286" s="12"/>
       <c r="I286" s="3"/>
       <c r="J286" s="3"/>
       <c r="K286" s="3"/>
@@ -5721,12 +5769,12 @@
     <row r="287" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A287" s="3"/>
       <c r="B287" s="3"/>
-      <c r="C287" s="3"/>
+      <c r="C287" s="16"/>
       <c r="D287" s="3"/>
       <c r="E287" s="6"/>
       <c r="F287" s="3"/>
       <c r="G287" s="3"/>
-      <c r="H287" s="3"/>
+      <c r="H287" s="12"/>
       <c r="I287" s="3"/>
       <c r="J287" s="3"/>
       <c r="K287" s="3"/>
@@ -5738,12 +5786,12 @@
     <row r="288" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A288" s="3"/>
       <c r="B288" s="3"/>
-      <c r="C288" s="3"/>
+      <c r="C288" s="16"/>
       <c r="D288" s="3"/>
       <c r="E288" s="6"/>
       <c r="F288" s="3"/>
       <c r="G288" s="3"/>
-      <c r="H288" s="3"/>
+      <c r="H288" s="12"/>
       <c r="I288" s="3"/>
       <c r="J288" s="3"/>
       <c r="K288" s="3"/>
@@ -5755,12 +5803,12 @@
     <row r="289" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A289" s="3"/>
       <c r="B289" s="3"/>
-      <c r="C289" s="3"/>
+      <c r="C289" s="16"/>
       <c r="D289" s="3"/>
       <c r="E289" s="6"/>
       <c r="F289" s="3"/>
       <c r="G289" s="3"/>
-      <c r="H289" s="3"/>
+      <c r="H289" s="12"/>
       <c r="I289" s="3"/>
       <c r="J289" s="3"/>
       <c r="K289" s="3"/>
@@ -5772,12 +5820,12 @@
     <row r="290" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A290" s="3"/>
       <c r="B290" s="3"/>
-      <c r="C290" s="3"/>
+      <c r="C290" s="16"/>
       <c r="D290" s="3"/>
       <c r="E290" s="6"/>
       <c r="F290" s="3"/>
       <c r="G290" s="3"/>
-      <c r="H290" s="3"/>
+      <c r="H290" s="12"/>
       <c r="I290" s="3"/>
       <c r="J290" s="3"/>
       <c r="K290" s="3"/>
@@ -5789,12 +5837,12 @@
     <row r="291" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A291" s="3"/>
       <c r="B291" s="3"/>
-      <c r="C291" s="3"/>
+      <c r="C291" s="16"/>
       <c r="D291" s="3"/>
       <c r="E291" s="6"/>
       <c r="F291" s="3"/>
       <c r="G291" s="3"/>
-      <c r="H291" s="3"/>
+      <c r="H291" s="12"/>
       <c r="I291" s="3"/>
       <c r="J291" s="3"/>
       <c r="K291" s="3"/>
@@ -5806,12 +5854,12 @@
     <row r="292" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A292" s="3"/>
       <c r="B292" s="3"/>
-      <c r="C292" s="3"/>
+      <c r="C292" s="16"/>
       <c r="D292" s="3"/>
       <c r="E292" s="6"/>
       <c r="F292" s="3"/>
       <c r="G292" s="3"/>
-      <c r="H292" s="3"/>
+      <c r="H292" s="12"/>
       <c r="I292" s="3"/>
       <c r="J292" s="3"/>
       <c r="K292" s="3"/>
@@ -5823,12 +5871,12 @@
     <row r="293" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A293" s="3"/>
       <c r="B293" s="3"/>
-      <c r="C293" s="3"/>
+      <c r="C293" s="16"/>
       <c r="D293" s="3"/>
       <c r="E293" s="6"/>
       <c r="F293" s="3"/>
       <c r="G293" s="3"/>
-      <c r="H293" s="3"/>
+      <c r="H293" s="12"/>
       <c r="I293" s="3"/>
       <c r="J293" s="3"/>
       <c r="K293" s="3"/>
@@ -5840,12 +5888,12 @@
     <row r="294" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A294" s="3"/>
       <c r="B294" s="3"/>
-      <c r="C294" s="3"/>
+      <c r="C294" s="16"/>
       <c r="D294" s="3"/>
       <c r="E294" s="6"/>
       <c r="F294" s="3"/>
       <c r="G294" s="3"/>
-      <c r="H294" s="3"/>
+      <c r="H294" s="12"/>
       <c r="I294" s="3"/>
       <c r="J294" s="3"/>
       <c r="K294" s="3"/>
@@ -5857,12 +5905,12 @@
     <row r="295" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A295" s="3"/>
       <c r="B295" s="3"/>
-      <c r="C295" s="3"/>
+      <c r="C295" s="16"/>
       <c r="D295" s="3"/>
       <c r="E295" s="6"/>
       <c r="F295" s="3"/>
       <c r="G295" s="3"/>
-      <c r="H295" s="3"/>
+      <c r="H295" s="12"/>
       <c r="I295" s="3"/>
       <c r="J295" s="3"/>
       <c r="K295" s="3"/>
@@ -5874,12 +5922,12 @@
     <row r="296" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A296" s="3"/>
       <c r="B296" s="3"/>
-      <c r="C296" s="3"/>
+      <c r="C296" s="16"/>
       <c r="D296" s="3"/>
       <c r="E296" s="6"/>
       <c r="F296" s="3"/>
       <c r="G296" s="3"/>
-      <c r="H296" s="3"/>
+      <c r="H296" s="12"/>
       <c r="I296" s="3"/>
       <c r="J296" s="3"/>
       <c r="K296" s="3"/>
@@ -5891,12 +5939,12 @@
     <row r="297" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A297" s="3"/>
       <c r="B297" s="3"/>
-      <c r="C297" s="3"/>
+      <c r="C297" s="16"/>
       <c r="D297" s="3"/>
       <c r="E297" s="6"/>
       <c r="F297" s="3"/>
       <c r="G297" s="3"/>
-      <c r="H297" s="3"/>
+      <c r="H297" s="12"/>
       <c r="I297" s="3"/>
       <c r="J297" s="3"/>
       <c r="K297" s="3"/>
@@ -5908,12 +5956,12 @@
     <row r="298" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A298" s="3"/>
       <c r="B298" s="3"/>
-      <c r="C298" s="3"/>
+      <c r="C298" s="16"/>
       <c r="D298" s="3"/>
       <c r="E298" s="6"/>
       <c r="F298" s="3"/>
       <c r="G298" s="3"/>
-      <c r="H298" s="3"/>
+      <c r="H298" s="12"/>
       <c r="I298" s="3"/>
       <c r="J298" s="3"/>
       <c r="K298" s="3"/>
@@ -5925,12 +5973,12 @@
     <row r="299" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A299" s="3"/>
       <c r="B299" s="3"/>
-      <c r="C299" s="3"/>
+      <c r="C299" s="16"/>
       <c r="D299" s="3"/>
       <c r="E299" s="6"/>
       <c r="F299" s="3"/>
       <c r="G299" s="3"/>
-      <c r="H299" s="3"/>
+      <c r="H299" s="12"/>
       <c r="I299" s="3"/>
       <c r="J299" s="3"/>
       <c r="K299" s="3"/>
@@ -5942,12 +5990,12 @@
     <row r="300" spans="1:15" x14ac:dyDescent="0.75">
       <c r="A300" s="3"/>
       <c r="B300" s="3"/>
-      <c r="C300" s="3"/>
+      <c r="C300" s="16"/>
       <c r="D300" s="3"/>
       <c r="E300" s="6"/>
       <c r="F300" s="3"/>
       <c r="G300" s="3"/>
-      <c r="H300" s="3"/>
+      <c r="H300" s="12"/>
       <c r="I300" s="3"/>
       <c r="J300" s="3"/>
       <c r="K300" s="3"/>
@@ -5958,5 +6006,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>